<commit_message>
Add Bloomz for Zeroshot
</commit_message>
<xml_diff>
--- a/SIB-200 languages - ACL.xlsx
+++ b/SIB-200 languages - ACL.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R205"/>
+  <dimension ref="A1:S205"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -524,6 +524,11 @@
           <t>F1 PolyLM-1.7b beam-search</t>
         </is>
       </c>
+      <c r="S1" s="1" t="inlineStr">
+        <is>
+          <t>F1 Bloomz-560M beam-search</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -594,6 +599,9 @@
       <c r="R2" t="n">
         <v>0.04656862745098039</v>
       </c>
+      <c r="S2" t="n">
+        <v>0.09070043103448276</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -664,6 +672,9 @@
       <c r="R3" t="n">
         <v>0.116461849162742</v>
       </c>
+      <c r="S3" t="n">
+        <v>0.3683862836593088</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -728,6 +739,9 @@
       <c r="R4" t="n">
         <v>0.1289839632211324</v>
       </c>
+      <c r="S4" t="n">
+        <v>0.3907859603789836</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -792,6 +806,9 @@
       <c r="R5" t="n">
         <v>0.08032407407407408</v>
       </c>
+      <c r="S5" t="n">
+        <v>0.4011704460054532</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -856,6 +873,9 @@
       <c r="R6" t="n">
         <v>0.06823489438271074</v>
       </c>
+      <c r="S6" t="n">
+        <v>0.3734657155709787</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -931,6 +951,9 @@
       </c>
       <c r="R7" t="n">
         <v>0.07299462924462925</v>
+      </c>
+      <c r="S7" t="n">
+        <v>0.3117627140301559</v>
       </c>
     </row>
     <row r="8">
@@ -996,6 +1019,9 @@
       <c r="R8" t="n">
         <v>0.11784510974201</v>
       </c>
+      <c r="S8" t="n">
+        <v>0.3540195576780942</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -1072,6 +1098,9 @@
       <c r="R9" t="n">
         <v>0.04883003242314152</v>
       </c>
+      <c r="S9" t="n">
+        <v>0.296255737600408</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -1140,6 +1169,9 @@
       <c r="R10" t="n">
         <v>0.0432999348321929</v>
       </c>
+      <c r="S10" t="n">
+        <v>0.3093343084953823</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -1215,6 +1247,9 @@
       </c>
       <c r="R11" t="n">
         <v>0.03770949720670392</v>
+      </c>
+      <c r="S11" t="n">
+        <v>0.08756627522527154</v>
       </c>
     </row>
     <row r="12">
@@ -1280,6 +1315,9 @@
       <c r="R12" t="n">
         <v>0.1290329167687658</v>
       </c>
+      <c r="S12" t="n">
+        <v>0.3965951236852023</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -1346,6 +1384,9 @@
       <c r="R13" t="n">
         <v>0.09491891499435269</v>
       </c>
+      <c r="S13" t="n">
+        <v>0.3767832752299624</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -1410,6 +1451,9 @@
       <c r="R14" t="n">
         <v>0.04437229437229437</v>
       </c>
+      <c r="S14" t="n">
+        <v>0.1955820956146577</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -1474,6 +1518,9 @@
       <c r="R15" t="n">
         <v>0.09921926292292205</v>
       </c>
+      <c r="S15" t="n">
+        <v>0.3714567361946708</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -1538,6 +1585,9 @@
       <c r="R16" t="n">
         <v>0.1207316282537521</v>
       </c>
+      <c r="S16" t="n">
+        <v>0.3701715169520402</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -1600,6 +1650,9 @@
       <c r="R17" t="n">
         <v>0.118021230281441</v>
       </c>
+      <c r="S17" t="n">
+        <v>0.3893145416379112</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -1677,6 +1730,9 @@
       </c>
       <c r="R18" t="n">
         <v>0</v>
+      </c>
+      <c r="S18" t="n">
+        <v>0.3557140934176874</v>
       </c>
     </row>
     <row r="19">
@@ -1748,6 +1804,9 @@
       <c r="R19" t="n">
         <v>0.1046194546194546</v>
       </c>
+      <c r="S19" t="n">
+        <v>0.4531567683844723</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -1818,6 +1877,9 @@
       <c r="R20" t="n">
         <v>0.03849865527606391</v>
       </c>
+      <c r="S20" t="n">
+        <v>0.3255910559257016</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -1880,6 +1942,9 @@
       <c r="R21" t="n">
         <v>0.05352633477633478</v>
       </c>
+      <c r="S21" t="n">
+        <v>0.2678994640899403</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -1942,6 +2007,9 @@
       <c r="R22" t="n">
         <v>0.03730158730158731</v>
       </c>
+      <c r="S22" t="n">
+        <v>0.1605946684894053</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -2006,6 +2074,9 @@
       <c r="R23" t="n">
         <v>0.0552703373015873</v>
       </c>
+      <c r="S23" t="n">
+        <v>0.2365546218487395</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -2080,6 +2151,9 @@
       <c r="R24" t="n">
         <v>0</v>
       </c>
+      <c r="S24" t="n">
+        <v>0.1172363379713652</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -2155,6 +2229,9 @@
       </c>
       <c r="R25" t="n">
         <v>0.02939322301024429</v>
+      </c>
+      <c r="S25" t="n">
+        <v>0.2505002470355731</v>
       </c>
     </row>
     <row r="26">
@@ -2226,6 +2303,9 @@
       <c r="R26" t="n">
         <v>0.1072459991748637</v>
       </c>
+      <c r="S26" t="n">
+        <v>0.370645915881345</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -2301,6 +2381,9 @@
       </c>
       <c r="R27" t="n">
         <v>0.06901808578745197</v>
+      </c>
+      <c r="S27" t="n">
+        <v>0.08881038448899112</v>
       </c>
     </row>
     <row r="28">
@@ -2372,6 +2455,9 @@
       <c r="R28" t="n">
         <v>0.06022809185459788</v>
       </c>
+      <c r="S28" t="n">
+        <v>0.2751988777521063</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -2449,6 +2535,9 @@
       </c>
       <c r="R29" t="n">
         <v>0</v>
+      </c>
+      <c r="S29" t="n">
+        <v>0.3638318742130999</v>
       </c>
     </row>
     <row r="30">
@@ -2520,6 +2609,9 @@
       <c r="R30" t="n">
         <v>0.02599379132398</v>
       </c>
+      <c r="S30" t="n">
+        <v>0.301610305958132</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -2582,6 +2674,9 @@
       <c r="R31" t="n">
         <v>0.03203125</v>
       </c>
+      <c r="S31" t="n">
+        <v>0.09680952380952382</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -2644,6 +2739,9 @@
       <c r="R32" t="n">
         <v>0.0841221752630671</v>
       </c>
+      <c r="S32" t="n">
+        <v>0.3727749339952695</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -2718,6 +2816,9 @@
       <c r="R33" t="n">
         <v>0.03235294117647058</v>
       </c>
+      <c r="S33" t="n">
+        <v>0.05386317222600408</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -2793,6 +2894,9 @@
       </c>
       <c r="R34" t="n">
         <v>0.07151783638356529</v>
+      </c>
+      <c r="S34" t="n">
+        <v>0.3117566663297645</v>
       </c>
     </row>
     <row r="35">
@@ -2864,6 +2968,9 @@
       <c r="R35" t="n">
         <v>0.08899496775412413</v>
       </c>
+      <c r="S35" t="n">
+        <v>0.3423585884795018</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -2940,6 +3047,9 @@
       <c r="R36" t="n">
         <v>0.05846508563899869</v>
       </c>
+      <c r="S36" t="n">
+        <v>0.146856097354824</v>
+      </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -3017,6 +3127,9 @@
       </c>
       <c r="R37" t="n">
         <v>0.06680341055341055</v>
+      </c>
+      <c r="S37" t="n">
+        <v>0.456802037335402</v>
       </c>
     </row>
     <row r="38">
@@ -3088,6 +3201,9 @@
       <c r="R38" t="n">
         <v>0.09252694138660329</v>
       </c>
+      <c r="S38" t="n">
+        <v>0.3317517654669598</v>
+      </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -3163,6 +3279,9 @@
       </c>
       <c r="R39" t="n">
         <v>0.04956501831501831</v>
+      </c>
+      <c r="S39" t="n">
+        <v>0.3015296708940777</v>
       </c>
     </row>
     <row r="40">
@@ -3228,6 +3347,9 @@
       <c r="R40" t="n">
         <v>0.06088033984731575</v>
       </c>
+      <c r="S40" t="n">
+        <v>0.2627459685417076</v>
+      </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -3290,6 +3412,9 @@
       <c r="R41" t="n">
         <v>0.02228163992869875</v>
       </c>
+      <c r="S41" t="n">
+        <v>0.1345762516760939</v>
+      </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
@@ -3360,6 +3485,9 @@
       <c r="R42" t="n">
         <v>0.05557141648690945</v>
       </c>
+      <c r="S42" t="n">
+        <v>0.2505593889923849</v>
+      </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
@@ -3436,6 +3564,9 @@
       <c r="R43" t="n">
         <v>0.06854777167277168</v>
       </c>
+      <c r="S43" t="n">
+        <v>0.242181583404605</v>
+      </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
@@ -3512,6 +3643,9 @@
       <c r="R44" t="n">
         <v>0.119688374014747</v>
       </c>
+      <c r="S44" t="n">
+        <v>0.3224900059138657</v>
+      </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
@@ -3587,6 +3721,9 @@
       </c>
       <c r="R45" t="n">
         <v>0.1172670707627313</v>
+      </c>
+      <c r="S45" t="n">
+        <v>0.3425158540084919</v>
       </c>
     </row>
     <row r="46">
@@ -3650,6 +3787,9 @@
       <c r="R46" t="n">
         <v>0.05423806458853953</v>
       </c>
+      <c r="S46" t="n">
+        <v>0.2628034523702301</v>
+      </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
@@ -3720,6 +3860,9 @@
       <c r="R47" t="n">
         <v>0.0756990446810171</v>
       </c>
+      <c r="S47" t="n">
+        <v>0.2761562232475772</v>
+      </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
@@ -3794,6 +3937,9 @@
       <c r="R48" t="n">
         <v>0.03260869565217392</v>
       </c>
+      <c r="S48" t="n">
+        <v>0.04028925619834711</v>
+      </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
@@ -3870,6 +4016,9 @@
       <c r="R49" t="n">
         <v>0.02892561983471074</v>
       </c>
+      <c r="S49" t="n">
+        <v>0.1420755395426053</v>
+      </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
@@ -3947,6 +4096,9 @@
       </c>
       <c r="R50" t="n">
         <v>0.05380150539550035</v>
+      </c>
+      <c r="S50" t="n">
+        <v>0.4202765820303225</v>
       </c>
     </row>
     <row r="51">
@@ -4024,6 +4176,9 @@
       <c r="R51" t="n">
         <v>0.06616844116844117</v>
       </c>
+      <c r="S51" t="n">
+        <v>0.3413712145757019</v>
+      </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
@@ -4100,6 +4255,9 @@
       <c r="R52" t="n">
         <v>0.09298962531721153</v>
       </c>
+      <c r="S52" t="n">
+        <v>0.2791354712754004</v>
+      </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
@@ -4177,6 +4335,9 @@
       </c>
       <c r="R53" t="n">
         <v>0.06090346586395752</v>
+      </c>
+      <c r="S53" t="n">
+        <v>0.4030589001298249</v>
       </c>
     </row>
     <row r="54">
@@ -4252,6 +4413,9 @@
       <c r="R54" t="n">
         <v>0.04545940170940171</v>
       </c>
+      <c r="S54" t="n">
+        <v>0.2631649818013417</v>
+      </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
@@ -4326,6 +4490,9 @@
       <c r="R55" t="n">
         <v>0.06445645451856633</v>
       </c>
+      <c r="S55" t="n">
+        <v>0.2299949733388913</v>
+      </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
@@ -4400,6 +4567,9 @@
       <c r="R56" t="n">
         <v>0.05947871572871574</v>
       </c>
+      <c r="S56" t="n">
+        <v>0.2531380518865041</v>
+      </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
@@ -4476,6 +4646,9 @@
       <c r="R57" t="n">
         <v>0.05425324675324676</v>
       </c>
+      <c r="S57" t="n">
+        <v>0.2808818362857735</v>
+      </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
@@ -4548,6 +4721,9 @@
       <c r="R58" t="n">
         <v>0.02544544123602156</v>
       </c>
+      <c r="S58" t="n">
+        <v>0.2701452957327042</v>
+      </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
@@ -4625,6 +4801,9 @@
       </c>
       <c r="R59" t="n">
         <v>0.1043923269201636</v>
+      </c>
+      <c r="S59" t="n">
+        <v>0.4293815696579533</v>
       </c>
     </row>
     <row r="60">
@@ -4696,6 +4875,9 @@
       <c r="R60" t="n">
         <v>0.0434939456678587</v>
       </c>
+      <c r="S60" t="n">
+        <v>0.3718636467653506</v>
+      </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
@@ -4758,6 +4940,9 @@
       <c r="R61" t="n">
         <v>0.08753997405077615</v>
       </c>
+      <c r="S61" t="n">
+        <v>0.3035802676530116</v>
+      </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
@@ -4826,6 +5011,9 @@
       <c r="R62" t="n">
         <v>0.06228913630229418</v>
       </c>
+      <c r="S62" t="n">
+        <v>0.1840219030756115</v>
+      </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
@@ -4902,6 +5090,9 @@
       <c r="R63" t="n">
         <v>0.07772533973574365</v>
       </c>
+      <c r="S63" t="n">
+        <v>0.2250104733975702</v>
+      </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
@@ -4978,6 +5169,9 @@
       <c r="R64" t="n">
         <v>0.0531873118373402</v>
       </c>
+      <c r="S64" t="n">
+        <v>0.2271187258687259</v>
+      </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
@@ -5053,6 +5247,9 @@
       </c>
       <c r="R65" t="n">
         <v>0.1161213110295118</v>
+      </c>
+      <c r="S65" t="n">
+        <v>0.422134169961877</v>
       </c>
     </row>
     <row r="66">
@@ -5128,6 +5325,9 @@
       <c r="R66" t="n">
         <v>0.05536522301228183</v>
       </c>
+      <c r="S66" t="n">
+        <v>0.3150487080193367</v>
+      </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
@@ -5205,6 +5405,9 @@
       </c>
       <c r="R67" t="n">
         <v>0.008474576271186441</v>
+      </c>
+      <c r="S67" t="n">
+        <v>0.3302532177919711</v>
       </c>
     </row>
     <row r="68">
@@ -5280,6 +5483,9 @@
       <c r="R68" t="n">
         <v>0.07918320105820106</v>
       </c>
+      <c r="S68" t="n">
+        <v>0.2879818931128506</v>
+      </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
@@ -5356,6 +5562,9 @@
       <c r="R69" t="n">
         <v>0.04474194206446348</v>
       </c>
+      <c r="S69" t="n">
+        <v>0.3117668729737695</v>
+      </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
@@ -5432,6 +5641,9 @@
       <c r="R70" t="n">
         <v>0.06838050316788069</v>
       </c>
+      <c r="S70" t="n">
+        <v>0.100731316369465</v>
+      </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
@@ -5509,6 +5721,9 @@
       </c>
       <c r="R71" t="n">
         <v>0.006756756756756757</v>
+      </c>
+      <c r="S71" t="n">
+        <v>0.3254412159628695</v>
       </c>
     </row>
     <row r="72">
@@ -5574,6 +5789,9 @@
       <c r="R72" t="n">
         <v>0.02040816326530612</v>
       </c>
+      <c r="S72" t="n">
+        <v>0.2877494290652556</v>
+      </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
@@ -5650,6 +5868,9 @@
       <c r="R73" t="n">
         <v>0.07500769463390879</v>
       </c>
+      <c r="S73" t="n">
+        <v>0.2816965024110335</v>
+      </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
@@ -5726,6 +5947,9 @@
       <c r="R74" t="n">
         <v>0.0657846057986253</v>
       </c>
+      <c r="S74" t="n">
+        <v>0.28943290503387</v>
+      </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
@@ -5802,6 +6026,9 @@
       <c r="R75" t="n">
         <v>0.03483606557377049</v>
       </c>
+      <c r="S75" t="n">
+        <v>0.03859060402684564</v>
+      </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
@@ -5877,6 +6104,9 @@
       </c>
       <c r="R76" t="n">
         <v>0.1045085159405201</v>
+      </c>
+      <c r="S76" t="n">
+        <v>0.2735011441647597</v>
       </c>
     </row>
     <row r="77">
@@ -5948,6 +6178,9 @@
       <c r="R77" t="n">
         <v>0.07455071948134091</v>
       </c>
+      <c r="S77" t="n">
+        <v>0.3619225881294846</v>
+      </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
@@ -6025,6 +6258,9 @@
       </c>
       <c r="R78" t="n">
         <v>0.08981481481481482</v>
+      </c>
+      <c r="S78" t="n">
+        <v>0.4085303909989531</v>
       </c>
     </row>
     <row r="79">
@@ -6102,6 +6338,9 @@
       <c r="R79" t="n">
         <v>0.04743092824488173</v>
       </c>
+      <c r="S79" t="n">
+        <v>0.2289802925250098</v>
+      </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
@@ -6178,6 +6417,9 @@
       <c r="R80" t="n">
         <v>0.1105694980694981</v>
       </c>
+      <c r="S80" t="n">
+        <v>0.4039683680249718</v>
+      </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
@@ -6254,6 +6496,9 @@
       <c r="R81" t="n">
         <v>0.09582624500253337</v>
       </c>
+      <c r="S81" t="n">
+        <v>0.3947003214297173</v>
+      </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
@@ -6329,6 +6574,9 @@
       </c>
       <c r="R82" t="n">
         <v>0.06713497245385748</v>
+      </c>
+      <c r="S82" t="n">
+        <v>0.235208102041176</v>
       </c>
     </row>
     <row r="83">
@@ -6400,6 +6648,9 @@
       <c r="R83" t="n">
         <v>0.05896328048808147</v>
       </c>
+      <c r="S83" t="n">
+        <v>0.1238629862700229</v>
+      </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
@@ -6470,6 +6721,9 @@
       <c r="R84" t="n">
         <v>0.03052184466019418</v>
       </c>
+      <c r="S84" t="n">
+        <v>0.27211174487944</v>
+      </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
@@ -6540,6 +6794,9 @@
       <c r="R85" t="n">
         <v>0.05681818181818182</v>
       </c>
+      <c r="S85" t="n">
+        <v>0.2780394157159739</v>
+      </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
@@ -6617,6 +6874,9 @@
       </c>
       <c r="R86" t="n">
         <v>0.01285797779076564</v>
+      </c>
+      <c r="S86" t="n">
+        <v>0.3301407220242923</v>
       </c>
     </row>
     <row r="87">
@@ -6692,6 +6952,9 @@
       <c r="R87" t="n">
         <v>0.02598566308243727</v>
       </c>
+      <c r="S87" t="n">
+        <v>0.2494397759103641</v>
+      </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
@@ -6766,6 +7029,9 @@
       <c r="R88" t="n">
         <v>0.01985785953177258</v>
       </c>
+      <c r="S88" t="n">
+        <v>0.213216176939003</v>
+      </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
@@ -6842,6 +7108,9 @@
       <c r="R89" t="n">
         <v>0.01960784313725491</v>
       </c>
+      <c r="S89" t="n">
+        <v>0.1196394977511837</v>
+      </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
@@ -6917,6 +7186,9 @@
       </c>
       <c r="R90" t="n">
         <v>0.01744851258581236</v>
+      </c>
+      <c r="S90" t="n">
+        <v>0.1254913592810057</v>
       </c>
     </row>
     <row r="91">
@@ -6980,6 +7252,9 @@
       <c r="R91" t="n">
         <v>0.01507321274763135</v>
       </c>
+      <c r="S91" t="n">
+        <v>0.2805411160778968</v>
+      </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
@@ -7044,6 +7319,9 @@
       <c r="R92" t="n">
         <v>0.083774284535961</v>
       </c>
+      <c r="S92" t="n">
+        <v>0.3751131932583546</v>
+      </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
@@ -7112,6 +7390,9 @@
       <c r="R93" t="n">
         <v>0.03803483750292261</v>
       </c>
+      <c r="S93" t="n">
+        <v>0.08239831697054699</v>
+      </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
@@ -7188,6 +7469,9 @@
       <c r="R94" t="n">
         <v>0</v>
       </c>
+      <c r="S94" t="n">
+        <v>0.1809535756764793</v>
+      </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
@@ -7264,6 +7548,9 @@
       <c r="R95" t="n">
         <v>0.05827991452991452</v>
       </c>
+      <c r="S95" t="n">
+        <v>0.2829564048620851</v>
+      </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
@@ -7340,6 +7627,9 @@
       <c r="R96" t="n">
         <v>0.04777200237816287</v>
       </c>
+      <c r="S96" t="n">
+        <v>0.3233153896982801</v>
+      </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
@@ -7415,6 +7705,9 @@
       </c>
       <c r="R97" t="n">
         <v>0.02172904423136406</v>
+      </c>
+      <c r="S97" t="n">
+        <v>0.1321063396900866</v>
       </c>
     </row>
     <row r="98">
@@ -7486,6 +7779,9 @@
       <c r="R98" t="n">
         <v>0.06011085087570781</v>
       </c>
+      <c r="S98" t="n">
+        <v>0.2634822884887972</v>
+      </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
@@ -7553,6 +7849,9 @@
       </c>
       <c r="R99" t="n">
         <v>0.04640485016991042</v>
+      </c>
+      <c r="S99" t="n">
+        <v>0.2287671328469243</v>
       </c>
     </row>
     <row r="100">
@@ -7616,6 +7915,9 @@
       <c r="R100" t="n">
         <v>0.0302547770700637</v>
       </c>
+      <c r="S100" t="n">
+        <v>0.06261534877887079</v>
+      </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
@@ -7678,6 +7980,9 @@
       <c r="R101" t="n">
         <v>0.08740765347908205</v>
       </c>
+      <c r="S101" t="n">
+        <v>0.2957986484227619</v>
+      </c>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
@@ -7752,6 +8057,9 @@
       <c r="R102" t="n">
         <v>0.1035795418491021</v>
       </c>
+      <c r="S102" t="n">
+        <v>0.3358617947123999</v>
+      </c>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
@@ -7828,6 +8136,9 @@
       <c r="R103" t="n">
         <v>0.03728070175438596</v>
       </c>
+      <c r="S103" t="n">
+        <v>0.1331778206778207</v>
+      </c>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
@@ -7903,6 +8214,9 @@
       </c>
       <c r="R104" t="n">
         <v>0.0339265850945495</v>
+      </c>
+      <c r="S104" t="n">
+        <v>0.1798729979558371</v>
       </c>
     </row>
     <row r="105">
@@ -7966,6 +8280,9 @@
       <c r="R105" t="n">
         <v>0.09471677920473101</v>
       </c>
+      <c r="S105" t="n">
+        <v>0.3550461033219654</v>
+      </c>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
@@ -8040,6 +8357,9 @@
       <c r="R106" t="n">
         <v>0.0832019239464641</v>
       </c>
+      <c r="S106" t="n">
+        <v>0.3137721998016115</v>
+      </c>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
@@ -8116,6 +8436,9 @@
       <c r="R107" t="n">
         <v>0.1202591036414566</v>
       </c>
+      <c r="S107" t="n">
+        <v>0.341674852024036</v>
+      </c>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
@@ -8191,6 +8514,9 @@
       </c>
       <c r="R108" t="n">
         <v>0.035</v>
+      </c>
+      <c r="S108" t="n">
+        <v>0.2495034503621055</v>
       </c>
     </row>
     <row r="109">
@@ -8254,6 +8580,9 @@
       <c r="R109" t="n">
         <v>0.09746453873382344</v>
       </c>
+      <c r="S109" t="n">
+        <v>0.3199567088656211</v>
+      </c>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr">
@@ -8316,6 +8645,9 @@
       <c r="R110" t="n">
         <v>0.06451481791155704</v>
       </c>
+      <c r="S110" t="n">
+        <v>0.2696602365642613</v>
+      </c>
     </row>
     <row r="111">
       <c r="A111" t="inlineStr">
@@ -8390,6 +8722,9 @@
       <c r="R111" t="n">
         <v>0.1045088915034884</v>
       </c>
+      <c r="S111" t="n">
+        <v>0.3238945427830517</v>
+      </c>
     </row>
     <row r="112">
       <c r="A112" t="inlineStr">
@@ -8460,6 +8795,9 @@
       <c r="R112" t="n">
         <v>0.0807578262562398</v>
       </c>
+      <c r="S112" t="n">
+        <v>0.3209640284752728</v>
+      </c>
     </row>
     <row r="113">
       <c r="A113" t="inlineStr">
@@ -8535,6 +8873,9 @@
       </c>
       <c r="R113" t="n">
         <v>0.09996951542396673</v>
+      </c>
+      <c r="S113" t="n">
+        <v>0.2595320473136083</v>
       </c>
     </row>
     <row r="114">
@@ -8608,6 +8949,9 @@
       <c r="R114" t="n">
         <v>0.06117548537052229</v>
       </c>
+      <c r="S114" t="n">
+        <v>0.2609109931827034</v>
+      </c>
     </row>
     <row r="115">
       <c r="A115" t="inlineStr">
@@ -8678,6 +9022,9 @@
       <c r="R115" t="n">
         <v>0.07906480117820323</v>
       </c>
+      <c r="S115" t="n">
+        <v>0.3219597399003874</v>
+      </c>
     </row>
     <row r="116">
       <c r="A116" t="inlineStr">
@@ -8745,6 +9092,9 @@
       </c>
       <c r="R116" t="n">
         <v>0.02381627636874375</v>
+      </c>
+      <c r="S116" t="n">
+        <v>0.2656881766010174</v>
       </c>
     </row>
     <row r="117">
@@ -8816,6 +9166,9 @@
       <c r="R117" t="n">
         <v>0.03125</v>
       </c>
+      <c r="S117" t="n">
+        <v>0.3248954599761051</v>
+      </c>
     </row>
     <row r="118">
       <c r="A118" t="inlineStr">
@@ -8886,6 +9239,9 @@
       <c r="R118" t="n">
         <v>0.02</v>
       </c>
+      <c r="S118" t="n">
+        <v>0.3459200185834674</v>
+      </c>
     </row>
     <row r="119">
       <c r="A119" t="inlineStr">
@@ -8964,6 +9320,9 @@
       <c r="R119" t="n">
         <v>0.0275</v>
       </c>
+      <c r="S119" t="n">
+        <v>0.3500042593784162</v>
+      </c>
     </row>
     <row r="120">
       <c r="A120" t="inlineStr">
@@ -9041,6 +9400,9 @@
       </c>
       <c r="R120" t="n">
         <v>0</v>
+      </c>
+      <c r="S120" t="n">
+        <v>0.3194923972298946</v>
       </c>
     </row>
     <row r="121">
@@ -9112,6 +9474,9 @@
       <c r="R121" t="n">
         <v>0.04109149277688603</v>
       </c>
+      <c r="S121" t="n">
+        <v>0.1132762943109637</v>
+      </c>
     </row>
     <row r="122">
       <c r="A122" t="inlineStr">
@@ -9182,6 +9547,9 @@
       <c r="R122" t="n">
         <v>0.1137653563297978</v>
       </c>
+      <c r="S122" t="n">
+        <v>0.3645563801085215</v>
+      </c>
     </row>
     <row r="123">
       <c r="A123" t="inlineStr">
@@ -9257,6 +9625,9 @@
       </c>
       <c r="R123" t="n">
         <v>0.07273056255081199</v>
+      </c>
+      <c r="S123" t="n">
+        <v>0.1299435028248588</v>
       </c>
     </row>
     <row r="124">
@@ -9332,6 +9703,9 @@
       <c r="R124" t="n">
         <v>0.03348152264517922</v>
       </c>
+      <c r="S124" t="n">
+        <v>0.3001043480924582</v>
+      </c>
     </row>
     <row r="125">
       <c r="A125" t="inlineStr">
@@ -9404,6 +9778,9 @@
       <c r="R125" t="n">
         <v>0</v>
       </c>
+      <c r="S125" t="n">
+        <v>0.1534391534391534</v>
+      </c>
     </row>
     <row r="126">
       <c r="A126" t="inlineStr">
@@ -9474,6 +9851,9 @@
       <c r="R126" t="n">
         <v>0.02124907612712491</v>
       </c>
+      <c r="S126" t="n">
+        <v>0.2714341887843866</v>
+      </c>
     </row>
     <row r="127">
       <c r="A127" t="inlineStr">
@@ -9548,6 +9928,9 @@
       <c r="R127" t="n">
         <v>0.05235192739303079</v>
       </c>
+      <c r="S127" t="n">
+        <v>0.2440288421170891</v>
+      </c>
     </row>
     <row r="128">
       <c r="A128" t="inlineStr">
@@ -9624,6 +10007,9 @@
       <c r="R128" t="n">
         <v>0.06453099233679309</v>
       </c>
+      <c r="S128" t="n">
+        <v>0.1114580732562118</v>
+      </c>
     </row>
     <row r="129">
       <c r="A129" t="inlineStr">
@@ -9699,6 +10085,9 @@
       </c>
       <c r="R129" t="n">
         <v>0.07872691034455739</v>
+      </c>
+      <c r="S129" t="n">
+        <v>0.3339136302294197</v>
       </c>
     </row>
     <row r="130">
@@ -9774,6 +10163,9 @@
       <c r="R130" t="n">
         <v>0.1107526763791345</v>
       </c>
+      <c r="S130" t="n">
+        <v>0.2966895455734742</v>
+      </c>
     </row>
     <row r="131">
       <c r="A131" t="inlineStr">
@@ -9848,6 +10240,9 @@
       <c r="R131" t="n">
         <v>0.1151382766831962</v>
       </c>
+      <c r="S131" t="n">
+        <v>0.2908797131821687</v>
+      </c>
     </row>
     <row r="132">
       <c r="A132" t="inlineStr">
@@ -9918,6 +10313,9 @@
       <c r="R132" t="n">
         <v>0.03194915254237288</v>
       </c>
+      <c r="S132" t="n">
+        <v>0.3388694366635543</v>
+      </c>
     </row>
     <row r="133">
       <c r="A133" t="inlineStr">
@@ -9989,6 +10387,9 @@
       </c>
       <c r="R133" t="n">
         <v>0.06636936791298122</v>
+      </c>
+      <c r="S133" t="n">
+        <v>0.2745280691848198</v>
       </c>
     </row>
     <row r="134">
@@ -10052,6 +10453,9 @@
       <c r="R134" t="n">
         <v>0.03057747489239598</v>
       </c>
+      <c r="S134" t="n">
+        <v>0.1905942675983437</v>
+      </c>
     </row>
     <row r="135">
       <c r="A135" t="inlineStr">
@@ -10127,6 +10531,9 @@
       </c>
       <c r="R135" t="n">
         <v>0.06470494111623143</v>
+      </c>
+      <c r="S135" t="n">
+        <v>0.2919585162440262</v>
       </c>
     </row>
     <row r="136">
@@ -10202,6 +10609,9 @@
       <c r="R136" t="n">
         <v>0.09065745909038381</v>
       </c>
+      <c r="S136" t="n">
+        <v>0.450389721832541</v>
+      </c>
     </row>
     <row r="137">
       <c r="A137" t="inlineStr">
@@ -10271,6 +10681,9 @@
       </c>
       <c r="R137" t="n">
         <v>0.004545454545454545</v>
+      </c>
+      <c r="S137" t="n">
+        <v>0.3196635791744487</v>
       </c>
     </row>
     <row r="138">
@@ -10342,6 +10755,9 @@
       <c r="R138" t="n">
         <v>0.08680482990827819</v>
       </c>
+      <c r="S138" t="n">
+        <v>0.3484545291839161</v>
+      </c>
     </row>
     <row r="139">
       <c r="A139" t="inlineStr">
@@ -10419,6 +10835,9 @@
       </c>
       <c r="R139" t="n">
         <v>0</v>
+      </c>
+      <c r="S139" t="n">
+        <v>0.3178021978021978</v>
       </c>
     </row>
     <row r="140">
@@ -10490,6 +10909,9 @@
       <c r="R140" t="n">
         <v>0.1064993784264799</v>
       </c>
+      <c r="S140" t="n">
+        <v>0.3956769954183747</v>
+      </c>
     </row>
     <row r="141">
       <c r="A141" t="inlineStr">
@@ -10558,6 +10980,9 @@
       <c r="R141" t="n">
         <v>0.04970760233918128</v>
       </c>
+      <c r="S141" t="n">
+        <v>0.191105808352049</v>
+      </c>
     </row>
     <row r="142">
       <c r="A142" t="inlineStr">
@@ -10625,6 +11050,9 @@
       </c>
       <c r="R142" t="n">
         <v>0.03785555528565876</v>
+      </c>
+      <c r="S142" t="n">
+        <v>0.2707260579313739</v>
       </c>
     </row>
     <row r="143">
@@ -10688,6 +11116,9 @@
       <c r="R143" t="n">
         <v>0.07430048547343068</v>
       </c>
+      <c r="S143" t="n">
+        <v>0.3421073163720223</v>
+      </c>
     </row>
     <row r="144">
       <c r="A144" t="inlineStr">
@@ -10764,6 +11195,9 @@
       <c r="R144" t="n">
         <v>0.08607824106909552</v>
       </c>
+      <c r="S144" t="n">
+        <v>0.281365443302563</v>
+      </c>
     </row>
     <row r="145">
       <c r="A145" t="inlineStr">
@@ -10841,6 +11275,9 @@
       </c>
       <c r="R145" t="n">
         <v>0.1169253147464157</v>
+      </c>
+      <c r="S145" t="n">
+        <v>0.4133212858637307</v>
       </c>
     </row>
     <row r="146">
@@ -10904,6 +11341,9 @@
       <c r="R146" t="n">
         <v>0.05448480355819126</v>
       </c>
+      <c r="S146" t="n">
+        <v>0.244881538290351</v>
+      </c>
     </row>
     <row r="147">
       <c r="A147" t="inlineStr">
@@ -10966,6 +11406,9 @@
       <c r="R147" t="n">
         <v>0.04315872403369991</v>
       </c>
+      <c r="S147" t="n">
+        <v>0.3241471415309218</v>
+      </c>
     </row>
     <row r="148">
       <c r="A148" t="inlineStr">
@@ -11042,6 +11485,9 @@
       <c r="R148" t="n">
         <v>0.06639758765358106</v>
       </c>
+      <c r="S148" t="n">
+        <v>0.3759947104901882</v>
+      </c>
     </row>
     <row r="149">
       <c r="A149" t="inlineStr">
@@ -11118,6 +11564,9 @@
       <c r="R149" t="n">
         <v>0.07208325440581705</v>
       </c>
+      <c r="S149" t="n">
+        <v>0.3062924735111436</v>
+      </c>
     </row>
     <row r="150">
       <c r="A150" t="inlineStr">
@@ -11193,6 +11642,9 @@
       </c>
       <c r="R150" t="n">
         <v>0.0903130946203079</v>
+      </c>
+      <c r="S150" t="n">
+        <v>0.1757912176390437</v>
       </c>
     </row>
     <row r="151">
@@ -11268,6 +11720,9 @@
       <c r="R151" t="n">
         <v>0.05698005698005698</v>
       </c>
+      <c r="S151" t="n">
+        <v>0.286403825888414</v>
+      </c>
     </row>
     <row r="152">
       <c r="A152" t="inlineStr">
@@ -11343,6 +11798,9 @@
       </c>
       <c r="R152" t="n">
         <v>0.02528735632183908</v>
+      </c>
+      <c r="S152" t="n">
+        <v>0.271362380229575</v>
       </c>
     </row>
     <row r="153">
@@ -11414,6 +11872,9 @@
       <c r="R153" t="n">
         <v>0.04166666666666666</v>
       </c>
+      <c r="S153" t="n">
+        <v>0.04868951612903226</v>
+      </c>
     </row>
     <row r="154">
       <c r="A154" t="inlineStr">
@@ -11484,6 +11945,9 @@
       <c r="R154" t="n">
         <v>0.05838509316770187</v>
       </c>
+      <c r="S154" t="n">
+        <v>0.3029636273113897</v>
+      </c>
     </row>
     <row r="155">
       <c r="A155" t="inlineStr">
@@ -11554,6 +12018,9 @@
       <c r="R155" t="n">
         <v>0.06452991452991452</v>
       </c>
+      <c r="S155" t="n">
+        <v>0.2470174662106029</v>
+      </c>
     </row>
     <row r="156">
       <c r="A156" t="inlineStr">
@@ -11630,6 +12097,9 @@
       <c r="R156" t="n">
         <v>0.005681818181818182</v>
       </c>
+      <c r="S156" t="n">
+        <v>0.08347647828954491</v>
+      </c>
     </row>
     <row r="157">
       <c r="A157" t="inlineStr">
@@ -11706,6 +12176,9 @@
       <c r="R157" t="n">
         <v>0.05371223064885036</v>
       </c>
+      <c r="S157" t="n">
+        <v>0.3239355397611124</v>
+      </c>
     </row>
     <row r="158">
       <c r="A158" t="inlineStr">
@@ -11781,6 +12254,9 @@
       </c>
       <c r="R158" t="n">
         <v>0.06914578111946533</v>
+      </c>
+      <c r="S158" t="n">
+        <v>0.3125143935110596</v>
       </c>
     </row>
     <row r="159">
@@ -11856,6 +12332,9 @@
       <c r="R159" t="n">
         <v>0.03363095238095238</v>
       </c>
+      <c r="S159" t="n">
+        <v>0.2780813953488372</v>
+      </c>
     </row>
     <row r="160">
       <c r="A160" t="inlineStr">
@@ -11932,6 +12411,9 @@
       <c r="R160" t="n">
         <v>0.07692273526746851</v>
       </c>
+      <c r="S160" t="n">
+        <v>0.2875833960150123</v>
+      </c>
     </row>
     <row r="161">
       <c r="A161" t="inlineStr">
@@ -12008,6 +12490,9 @@
       <c r="R161" t="n">
         <v>0.01954341058457281</v>
       </c>
+      <c r="S161" t="n">
+        <v>0.1883932848930054</v>
+      </c>
     </row>
     <row r="162">
       <c r="A162" t="inlineStr">
@@ -12084,6 +12569,9 @@
       <c r="R162" t="n">
         <v>0.05202973698507558</v>
       </c>
+      <c r="S162" t="n">
+        <v>0.2496171533792287</v>
+      </c>
     </row>
     <row r="163">
       <c r="A163" t="inlineStr">
@@ -12160,6 +12648,9 @@
       <c r="R163" t="n">
         <v>0.05017212725546059</v>
       </c>
+      <c r="S163" t="n">
+        <v>0.301229913703318</v>
+      </c>
     </row>
     <row r="164">
       <c r="A164" t="inlineStr">
@@ -12237,6 +12728,9 @@
       </c>
       <c r="R164" t="n">
         <v>0.1399074926168522</v>
+      </c>
+      <c r="S164" t="n">
+        <v>0.4369411888896962</v>
       </c>
     </row>
     <row r="165">
@@ -12312,6 +12806,9 @@
       <c r="R165" t="n">
         <v>0.1088595930960038</v>
       </c>
+      <c r="S165" t="n">
+        <v>0.3729404404404404</v>
+      </c>
     </row>
     <row r="166">
       <c r="A166" t="inlineStr">
@@ -12387,6 +12884,9 @@
       </c>
       <c r="R166" t="n">
         <v>0.126178033436098</v>
+      </c>
+      <c r="S166" t="n">
+        <v>0.1511588167629157</v>
       </c>
     </row>
     <row r="167">
@@ -12462,6 +12962,9 @@
       <c r="R167" t="n">
         <v>0.0819451471456278</v>
       </c>
+      <c r="S167" t="n">
+        <v>0.2692744755244755</v>
+      </c>
     </row>
     <row r="168">
       <c r="A168" t="inlineStr">
@@ -12538,6 +13041,9 @@
       <c r="R168" t="n">
         <v>0.07520363408521304</v>
       </c>
+      <c r="S168" t="n">
+        <v>0.3775288126507639</v>
+      </c>
     </row>
     <row r="169">
       <c r="A169" t="inlineStr">
@@ -12614,6 +13120,9 @@
       <c r="R169" t="n">
         <v>0.1239348749654601</v>
       </c>
+      <c r="S169" t="n">
+        <v>0.2982500580728793</v>
+      </c>
     </row>
     <row r="170">
       <c r="A170" t="inlineStr">
@@ -12683,6 +13192,9 @@
       </c>
       <c r="R170" t="n">
         <v>0.07579153693213789</v>
+      </c>
+      <c r="S170" t="n">
+        <v>0.3351247048335514</v>
       </c>
     </row>
     <row r="171">
@@ -12746,6 +13258,9 @@
       <c r="R171" t="n">
         <v>0.07872941012475897</v>
       </c>
+      <c r="S171" t="n">
+        <v>0.2315814393939394</v>
+      </c>
     </row>
     <row r="172">
       <c r="A172" t="inlineStr">
@@ -12823,6 +13338,9 @@
       </c>
       <c r="R172" t="n">
         <v>0</v>
+      </c>
+      <c r="S172" t="n">
+        <v>0.310705841603398</v>
       </c>
     </row>
     <row r="173">
@@ -12886,6 +13404,9 @@
       <c r="R173" t="n">
         <v>0.05866682643952728</v>
       </c>
+      <c r="S173" t="n">
+        <v>0.2325446828689753</v>
+      </c>
     </row>
     <row r="174">
       <c r="A174" t="inlineStr">
@@ -12948,6 +13469,9 @@
       <c r="R174" t="n">
         <v>0.02040816326530612</v>
       </c>
+      <c r="S174" t="n">
+        <v>0.0405549130560489</v>
+      </c>
     </row>
     <row r="175">
       <c r="A175" t="inlineStr">
@@ -13022,6 +13546,9 @@
       <c r="R175" t="n">
         <v>0.01333570412517781</v>
       </c>
+      <c r="S175" t="n">
+        <v>0.1180874450415242</v>
+      </c>
     </row>
     <row r="176">
       <c r="A176" t="inlineStr">
@@ -13099,6 +13626,9 @@
       </c>
       <c r="R176" t="n">
         <v>0.01207590569292697</v>
+      </c>
+      <c r="S176" t="n">
+        <v>0.3414307238551444</v>
       </c>
     </row>
     <row r="177">
@@ -13174,6 +13704,9 @@
       <c r="R177" t="n">
         <v>0.02708510940608127</v>
       </c>
+      <c r="S177" t="n">
+        <v>0.1254240845200192</v>
+      </c>
     </row>
     <row r="178">
       <c r="A178" t="inlineStr">
@@ -13250,6 +13783,9 @@
       <c r="R178" t="n">
         <v>0.07931857500010667</v>
       </c>
+      <c r="S178" t="n">
+        <v>0.3253770295706729</v>
+      </c>
     </row>
     <row r="179">
       <c r="A179" t="inlineStr">
@@ -13325,6 +13861,9 @@
       </c>
       <c r="R179" t="n">
         <v>0.08429164612350548</v>
+      </c>
+      <c r="S179" t="n">
+        <v>0.1056126219331954</v>
       </c>
     </row>
     <row r="180">
@@ -13400,6 +13939,9 @@
       <c r="R180" t="n">
         <v>0.04411764705882353</v>
       </c>
+      <c r="S180" t="n">
+        <v>0.07669671000788023</v>
+      </c>
     </row>
     <row r="181">
       <c r="A181" t="inlineStr">
@@ -13470,6 +14012,9 @@
       <c r="R181" t="n">
         <v>0.07588803691331782</v>
       </c>
+      <c r="S181" t="n">
+        <v>0.3500054848897665</v>
+      </c>
     </row>
     <row r="182">
       <c r="A182" t="inlineStr">
@@ -13546,6 +14091,9 @@
       <c r="R182" t="n">
         <v>0.09012640991034415</v>
       </c>
+      <c r="S182" t="n">
+        <v>0.2755578250718032</v>
+      </c>
     </row>
     <row r="183">
       <c r="A183" t="inlineStr">
@@ -13621,6 +14169,9 @@
       </c>
       <c r="R183" t="n">
         <v>0.0617003367003367</v>
+      </c>
+      <c r="S183" t="n">
+        <v>0.2747765862527946</v>
       </c>
     </row>
     <row r="184">
@@ -13696,6 +14247,9 @@
       <c r="R184" t="n">
         <v>0.05019109658189511</v>
       </c>
+      <c r="S184" t="n">
+        <v>0.2512373497581082</v>
+      </c>
     </row>
     <row r="185">
       <c r="A185" t="inlineStr">
@@ -13768,6 +14322,9 @@
       <c r="R185" t="n">
         <v>0.07363351254480287</v>
       </c>
+      <c r="S185" t="n">
+        <v>0.2696115270205416</v>
+      </c>
     </row>
     <row r="186">
       <c r="A186" t="inlineStr">
@@ -13843,6 +14400,9 @@
       </c>
       <c r="R186" t="n">
         <v>0.03412700700931585</v>
+      </c>
+      <c r="S186" t="n">
+        <v>0.2623324646314222</v>
       </c>
     </row>
     <row r="187">
@@ -13918,6 +14478,9 @@
       <c r="R187" t="n">
         <v>0.04255106446020051</v>
       </c>
+      <c r="S187" t="n">
+        <v>0.2996831865706038</v>
+      </c>
     </row>
     <row r="188">
       <c r="A188" t="inlineStr">
@@ -13982,6 +14545,9 @@
       <c r="R188" t="n">
         <v>0.009615384615384614</v>
       </c>
+      <c r="S188" t="n">
+        <v>0.04738516878804649</v>
+      </c>
     </row>
     <row r="189">
       <c r="A189" t="inlineStr">
@@ -14058,6 +14624,9 @@
       <c r="R189" t="n">
         <v>0.0447806191561767</v>
       </c>
+      <c r="S189" t="n">
+        <v>0.09310055542698449</v>
+      </c>
     </row>
     <row r="190">
       <c r="A190" t="inlineStr">
@@ -14133,6 +14702,9 @@
       </c>
       <c r="R190" t="n">
         <v>0.06980056980056981</v>
+      </c>
+      <c r="S190" t="n">
+        <v>0.1099094953213683</v>
       </c>
     </row>
     <row r="191">
@@ -14204,6 +14776,9 @@
       <c r="R191" t="n">
         <v>0.05092817088788591</v>
       </c>
+      <c r="S191" t="n">
+        <v>0.2233161897529714</v>
+      </c>
     </row>
     <row r="192">
       <c r="A192" t="inlineStr">
@@ -14281,6 +14856,9 @@
       </c>
       <c r="R192" t="n">
         <v>0.01416122004357299</v>
+      </c>
+      <c r="S192" t="n">
+        <v>0.320144613947038</v>
       </c>
     </row>
     <row r="193">
@@ -14349,6 +14927,9 @@
       </c>
       <c r="R193" t="n">
         <v>0.07269790856451473</v>
+      </c>
+      <c r="S193" t="n">
+        <v>0.2548226409262225</v>
       </c>
     </row>
     <row r="194">
@@ -14412,6 +14993,9 @@
       <c r="R194" t="n">
         <v>0.07833333333333334</v>
       </c>
+      <c r="S194" t="n">
+        <v>0.3438971974563001</v>
+      </c>
     </row>
     <row r="195">
       <c r="A195" t="inlineStr">
@@ -14489,6 +15073,9 @@
       </c>
       <c r="R195" t="n">
         <v>0.09274741092922911</v>
+      </c>
+      <c r="S195" t="n">
+        <v>0.3237704939392229</v>
       </c>
     </row>
     <row r="196">
@@ -14560,6 +15147,9 @@
       <c r="R196" t="n">
         <v>0.09364492917506874</v>
       </c>
+      <c r="S196" t="n">
+        <v>0.3654845305159475</v>
+      </c>
     </row>
     <row r="197">
       <c r="A197" t="inlineStr">
@@ -14636,6 +15226,9 @@
       <c r="R197" t="n">
         <v>0.07019048984892616</v>
       </c>
+      <c r="S197" t="n">
+        <v>0.2976210233842759</v>
+      </c>
     </row>
     <row r="198">
       <c r="A198" t="inlineStr">
@@ -14713,6 +15306,9 @@
       </c>
       <c r="R198" t="n">
         <v>0.09793447586169104</v>
+      </c>
+      <c r="S198" t="n">
+        <v>0.2886705677495535</v>
       </c>
     </row>
     <row r="199">
@@ -14782,6 +15378,9 @@
       <c r="R199" t="n">
         <v>0.03378378378378379</v>
       </c>
+      <c r="S199" t="n">
+        <v>0.1213393519254198</v>
+      </c>
     </row>
     <row r="200">
       <c r="A200" t="inlineStr">
@@ -14857,6 +15456,9 @@
       </c>
       <c r="R200" t="n">
         <v>0.0506388959877332</v>
+      </c>
+      <c r="S200" t="n">
+        <v>0.2365736672807519</v>
       </c>
     </row>
     <row r="201">
@@ -14922,6 +15524,9 @@
       <c r="R201" t="n">
         <v>0.0579187678244282</v>
       </c>
+      <c r="S201" t="n">
+        <v>0.3084219194924347</v>
+      </c>
     </row>
     <row r="202">
       <c r="A202" t="inlineStr">
@@ -15000,6 +15605,9 @@
       <c r="R202" t="n">
         <v>0.07599955488060328</v>
       </c>
+      <c r="S202" t="n">
+        <v>0.2943820240646866</v>
+      </c>
     </row>
     <row r="203">
       <c r="A203" t="inlineStr">
@@ -15077,6 +15685,9 @@
       </c>
       <c r="R203" t="n">
         <v>0.09005952380952381</v>
+      </c>
+      <c r="S203" t="n">
+        <v>0.2806850160687845</v>
       </c>
     </row>
     <row r="204">
@@ -15146,6 +15757,9 @@
       <c r="R204" t="n">
         <v>0.0903265236886045</v>
       </c>
+      <c r="S204" t="n">
+        <v>0.4006585026958826</v>
+      </c>
     </row>
     <row r="205">
       <c r="A205" t="inlineStr">
@@ -15221,6 +15835,9 @@
       </c>
       <c r="R205" t="n">
         <v>0.07018808548009368</v>
+      </c>
+      <c r="S205" t="n">
+        <v>0.2735147900229422</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
2-shot results for bloomz
</commit_message>
<xml_diff>
--- a/SIB-200 languages - ACL.xlsx
+++ b/SIB-200 languages - ACL.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AO205"/>
+  <dimension ref="A1:AQ205"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -639,6 +639,16 @@
           <t>F1 bloomz-560m generate 2-shot</t>
         </is>
       </c>
+      <c r="AP1" s="1" t="inlineStr">
+        <is>
+          <t>F1 bloomz-3b generate 2-shot</t>
+        </is>
+      </c>
+      <c r="AQ1" s="1" t="inlineStr">
+        <is>
+          <t>F1 bloomz-7b1 generate 2-shot</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -758,6 +768,12 @@
       <c r="AM2" t="inlineStr"/>
       <c r="AN2" t="inlineStr"/>
       <c r="AO2" t="inlineStr"/>
+      <c r="AP2" t="n">
+        <v>0.06083094394782707</v>
+      </c>
+      <c r="AQ2" t="n">
+        <v>0.1058786624004015</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -875,6 +891,12 @@
       <c r="AM3" t="inlineStr"/>
       <c r="AN3" t="inlineStr"/>
       <c r="AO3" t="inlineStr"/>
+      <c r="AP3" t="n">
+        <v>0.4543890359417669</v>
+      </c>
+      <c r="AQ3" t="n">
+        <v>0.6354753707016061</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -986,6 +1008,12 @@
       <c r="AM4" t="inlineStr"/>
       <c r="AN4" t="inlineStr"/>
       <c r="AO4" t="inlineStr"/>
+      <c r="AP4" t="n">
+        <v>0.5809407376329083</v>
+      </c>
+      <c r="AQ4" t="n">
+        <v>0.704608896839062</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -1097,6 +1125,12 @@
       <c r="AM5" t="inlineStr"/>
       <c r="AN5" t="inlineStr"/>
       <c r="AO5" t="inlineStr"/>
+      <c r="AP5" t="n">
+        <v>0.5812318373769367</v>
+      </c>
+      <c r="AQ5" t="n">
+        <v>0.6632073393128336</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -1212,6 +1246,12 @@
       <c r="AM6" t="inlineStr"/>
       <c r="AN6" t="inlineStr"/>
       <c r="AO6" t="inlineStr"/>
+      <c r="AP6" t="n">
+        <v>0.1176902193851346</v>
+      </c>
+      <c r="AQ6" t="n">
+        <v>0.647663263939126</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -1335,6 +1375,12 @@
       <c r="AM7" t="inlineStr"/>
       <c r="AN7" t="inlineStr"/>
       <c r="AO7" t="inlineStr"/>
+      <c r="AP7" t="n">
+        <v>0.4596800609138635</v>
+      </c>
+      <c r="AQ7" t="n">
+        <v>0.6132178172620925</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -1446,6 +1492,12 @@
       <c r="AM8" t="inlineStr"/>
       <c r="AN8" t="inlineStr"/>
       <c r="AO8" t="inlineStr"/>
+      <c r="AP8" t="n">
+        <v>0.6557943596711581</v>
+      </c>
+      <c r="AQ8" t="n">
+        <v>0.7060015256068279</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -1573,6 +1625,12 @@
       <c r="AM9" t="inlineStr"/>
       <c r="AN9" t="inlineStr"/>
       <c r="AO9" t="inlineStr"/>
+      <c r="AP9" t="n">
+        <v>0.1952934566156846</v>
+      </c>
+      <c r="AQ9" t="n">
+        <v>0.5865106276692836</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -1686,6 +1744,12 @@
       <c r="AM10" t="inlineStr"/>
       <c r="AN10" t="inlineStr"/>
       <c r="AO10" t="inlineStr"/>
+      <c r="AP10" t="n">
+        <v>0.294143798712714</v>
+      </c>
+      <c r="AQ10" t="n">
+        <v>0.4585339513188016</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -1807,6 +1871,12 @@
       <c r="AM11" t="inlineStr"/>
       <c r="AN11" t="inlineStr"/>
       <c r="AO11" t="inlineStr"/>
+      <c r="AP11" t="n">
+        <v>0.06083094394782707</v>
+      </c>
+      <c r="AQ11" t="n">
+        <v>0.07732772691789085</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -1924,6 +1994,12 @@
       <c r="AM12" t="inlineStr"/>
       <c r="AN12" t="inlineStr"/>
       <c r="AO12" t="inlineStr"/>
+      <c r="AP12" t="n">
+        <v>0.643092775837103</v>
+      </c>
+      <c r="AQ12" t="n">
+        <v>0.709775592371401</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -2041,6 +2117,12 @@
       <c r="AM13" t="inlineStr"/>
       <c r="AN13" t="inlineStr"/>
       <c r="AO13" t="inlineStr"/>
+      <c r="AP13" t="n">
+        <v>0.5813027095701867</v>
+      </c>
+      <c r="AQ13" t="n">
+        <v>0.6870236313508317</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -2150,6 +2232,12 @@
       <c r="AM14" t="inlineStr"/>
       <c r="AN14" t="inlineStr"/>
       <c r="AO14" t="inlineStr"/>
+      <c r="AP14" t="n">
+        <v>0.1700364141791897</v>
+      </c>
+      <c r="AQ14" t="n">
+        <v>0.3010588526507779</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -2263,6 +2351,12 @@
       <c r="AM15" t="inlineStr"/>
       <c r="AN15" t="inlineStr"/>
       <c r="AO15" t="inlineStr"/>
+      <c r="AP15" t="n">
+        <v>0.5665604514670844</v>
+      </c>
+      <c r="AQ15" t="n">
+        <v>0.6878995908579876</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -2376,6 +2470,12 @@
       <c r="AM16" t="inlineStr"/>
       <c r="AN16" t="inlineStr"/>
       <c r="AO16" t="inlineStr"/>
+      <c r="AP16" t="n">
+        <v>0.17458103452135</v>
+      </c>
+      <c r="AQ16" t="n">
+        <v>0.7252509148804104</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -2485,6 +2585,12 @@
       <c r="AM17" t="inlineStr"/>
       <c r="AN17" t="inlineStr"/>
       <c r="AO17" t="inlineStr"/>
+      <c r="AP17" t="n">
+        <v>0.6076048785468712</v>
+      </c>
+      <c r="AQ17" t="n">
+        <v>0.7039906136966214</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -2608,6 +2714,12 @@
       <c r="AM18" t="inlineStr"/>
       <c r="AN18" t="inlineStr"/>
       <c r="AO18" t="inlineStr"/>
+      <c r="AP18" t="n">
+        <v>0.5896366199947842</v>
+      </c>
+      <c r="AQ18" t="n">
+        <v>0.6759906533457993</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -2727,6 +2839,12 @@
       <c r="AM19" t="inlineStr"/>
       <c r="AN19" t="inlineStr"/>
       <c r="AO19" t="inlineStr"/>
+      <c r="AP19" t="n">
+        <v>0.7032764416336652</v>
+      </c>
+      <c r="AQ19" t="n">
+        <v>0.7414368102203752</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -2844,6 +2962,12 @@
       <c r="AM20" t="inlineStr"/>
       <c r="AN20" t="inlineStr"/>
       <c r="AO20" t="inlineStr"/>
+      <c r="AP20" t="n">
+        <v>0.5377087322698338</v>
+      </c>
+      <c r="AQ20" t="n">
+        <v>0.6527953319514171</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -2955,6 +3079,12 @@
       <c r="AM21" t="inlineStr"/>
       <c r="AN21" t="inlineStr"/>
       <c r="AO21" t="inlineStr"/>
+      <c r="AP21" t="n">
+        <v>0.2405334041278742</v>
+      </c>
+      <c r="AQ21" t="n">
+        <v>0.3327277985172722</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -3064,6 +3194,12 @@
       <c r="AM22" t="inlineStr"/>
       <c r="AN22" t="inlineStr"/>
       <c r="AO22" t="inlineStr"/>
+      <c r="AP22" t="n">
+        <v>0.1436611089864326</v>
+      </c>
+      <c r="AQ22" t="n">
+        <v>0.3113160714775536</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -3173,6 +3309,12 @@
       <c r="AM23" t="inlineStr"/>
       <c r="AN23" t="inlineStr"/>
       <c r="AO23" t="inlineStr"/>
+      <c r="AP23" t="n">
+        <v>0.2129421042340768</v>
+      </c>
+      <c r="AQ23" t="n">
+        <v>0.4848028861287249</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -3298,6 +3440,12 @@
       <c r="AM24" t="inlineStr"/>
       <c r="AN24" t="inlineStr"/>
       <c r="AO24" t="inlineStr"/>
+      <c r="AP24" t="n">
+        <v>0.06083094394782707</v>
+      </c>
+      <c r="AQ24" t="n">
+        <v>0.1491485634585319</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -3423,6 +3571,12 @@
       <c r="AM25" t="inlineStr"/>
       <c r="AN25" t="inlineStr"/>
       <c r="AO25" t="inlineStr"/>
+      <c r="AP25" t="n">
+        <v>0.0962876782512168</v>
+      </c>
+      <c r="AQ25" t="n">
+        <v>0.4182667478876517</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -3544,6 +3698,12 @@
       <c r="AM26" t="inlineStr"/>
       <c r="AN26" t="inlineStr"/>
       <c r="AO26" t="inlineStr"/>
+      <c r="AP26" t="n">
+        <v>0.532367753338398</v>
+      </c>
+      <c r="AQ26" t="n">
+        <v>0.6599449322210391</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -3665,6 +3825,12 @@
       <c r="AM27" t="inlineStr"/>
       <c r="AN27" t="inlineStr"/>
       <c r="AO27" t="inlineStr"/>
+      <c r="AP27" t="n">
+        <v>0.06083094394782707</v>
+      </c>
+      <c r="AQ27" t="n">
+        <v>0.1874884298899561</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -3784,6 +3950,12 @@
       <c r="AM28" t="inlineStr"/>
       <c r="AN28" t="inlineStr"/>
       <c r="AO28" t="inlineStr"/>
+      <c r="AP28" t="n">
+        <v>0.3945959965553916</v>
+      </c>
+      <c r="AQ28" t="n">
+        <v>0.5414649484102599</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -3911,6 +4083,12 @@
       <c r="AM29" t="inlineStr"/>
       <c r="AN29" t="inlineStr"/>
       <c r="AO29" t="inlineStr"/>
+      <c r="AP29" t="n">
+        <v>0.623990326841007</v>
+      </c>
+      <c r="AQ29" t="n">
+        <v>0.6853388002711732</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -4030,6 +4208,12 @@
       <c r="AM30" t="inlineStr"/>
       <c r="AN30" t="inlineStr"/>
       <c r="AO30" t="inlineStr"/>
+      <c r="AP30" t="n">
+        <v>0.5412290939441454</v>
+      </c>
+      <c r="AQ30" t="n">
+        <v>0.6588846663392769</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -4139,6 +4323,12 @@
       <c r="AM31" t="inlineStr"/>
       <c r="AN31" t="inlineStr"/>
       <c r="AO31" t="inlineStr"/>
+      <c r="AP31" t="n">
+        <v>0.0468384074941452</v>
+      </c>
+      <c r="AQ31" t="n">
+        <v>0.0578075123529669</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -4248,6 +4438,12 @@
       <c r="AM32" t="inlineStr"/>
       <c r="AN32" t="inlineStr"/>
       <c r="AO32" t="inlineStr"/>
+      <c r="AP32" t="n">
+        <v>0.5405996209119283</v>
+      </c>
+      <c r="AQ32" t="n">
+        <v>0.6427473739115472</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -4369,6 +4565,12 @@
       <c r="AM33" t="inlineStr"/>
       <c r="AN33" t="inlineStr"/>
       <c r="AO33" t="inlineStr"/>
+      <c r="AP33" t="n">
+        <v>0.05973575712143929</v>
+      </c>
+      <c r="AQ33" t="n">
+        <v>0.1088871250685361</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -4494,6 +4696,12 @@
       <c r="AM34" t="inlineStr"/>
       <c r="AN34" t="inlineStr"/>
       <c r="AO34" t="inlineStr"/>
+      <c r="AP34" t="n">
+        <v>0.3747261906679359</v>
+      </c>
+      <c r="AQ34" t="n">
+        <v>0.5495698481412766</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -4611,6 +4819,12 @@
       <c r="AM35" t="inlineStr"/>
       <c r="AN35" t="inlineStr"/>
       <c r="AO35" t="inlineStr"/>
+      <c r="AP35" t="n">
+        <v>0.4326993588428699</v>
+      </c>
+      <c r="AQ35" t="n">
+        <v>0.5209321576070345</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -4736,6 +4950,12 @@
       <c r="AM36" t="inlineStr"/>
       <c r="AN36" t="inlineStr"/>
       <c r="AO36" t="inlineStr"/>
+      <c r="AP36" t="n">
+        <v>0.1774613481756339</v>
+      </c>
+      <c r="AQ36" t="n">
+        <v>0.4356462878239881</v>
+      </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -4863,6 +5083,12 @@
       <c r="AM37" t="inlineStr"/>
       <c r="AN37" t="inlineStr"/>
       <c r="AO37" t="inlineStr"/>
+      <c r="AP37" t="n">
+        <v>0.7023569408121055</v>
+      </c>
+      <c r="AQ37" t="n">
+        <v>0.6895431467227998</v>
+      </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -4986,6 +5212,12 @@
       <c r="AM38" t="inlineStr"/>
       <c r="AN38" t="inlineStr"/>
       <c r="AO38" t="inlineStr"/>
+      <c r="AP38" t="n">
+        <v>0.4770855864535236</v>
+      </c>
+      <c r="AQ38" t="n">
+        <v>0.5783569150490626</v>
+      </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -5109,6 +5341,12 @@
       <c r="AM39" t="inlineStr"/>
       <c r="AN39" t="inlineStr"/>
       <c r="AO39" t="inlineStr"/>
+      <c r="AP39" t="n">
+        <v>0.3424345095498524</v>
+      </c>
+      <c r="AQ39" t="n">
+        <v>0.5477760235860432</v>
+      </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -5220,6 +5458,12 @@
       <c r="AM40" t="inlineStr"/>
       <c r="AN40" t="inlineStr"/>
       <c r="AO40" t="inlineStr"/>
+      <c r="AP40" t="n">
+        <v>0.3358372101164342</v>
+      </c>
+      <c r="AQ40" t="n">
+        <v>0.425364639719004</v>
+      </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -5329,6 +5573,12 @@
       <c r="AM41" t="inlineStr"/>
       <c r="AN41" t="inlineStr"/>
       <c r="AO41" t="inlineStr"/>
+      <c r="AP41" t="n">
+        <v>0.04722550177095632</v>
+      </c>
+      <c r="AQ41" t="n">
+        <v>0.09230495496255788</v>
+      </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
@@ -5446,6 +5696,12 @@
       <c r="AM42" t="inlineStr"/>
       <c r="AN42" t="inlineStr"/>
       <c r="AO42" t="inlineStr"/>
+      <c r="AP42" t="n">
+        <v>0.2596332275972105</v>
+      </c>
+      <c r="AQ42" t="n">
+        <v>0.4550390042004783</v>
+      </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
@@ -5569,6 +5825,12 @@
       <c r="AM43" t="inlineStr"/>
       <c r="AN43" t="inlineStr"/>
       <c r="AO43" t="inlineStr"/>
+      <c r="AP43" t="n">
+        <v>0.2625888499146121</v>
+      </c>
+      <c r="AQ43" t="n">
+        <v>0.3702508515833238</v>
+      </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
@@ -5690,6 +5952,12 @@
       <c r="AM44" t="inlineStr"/>
       <c r="AN44" t="inlineStr"/>
       <c r="AO44" t="inlineStr"/>
+      <c r="AP44" t="n">
+        <v>0.4807236871550974</v>
+      </c>
+      <c r="AQ44" t="n">
+        <v>0.5943761081709388</v>
+      </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
@@ -5819,6 +6087,12 @@
       <c r="AM45" t="inlineStr"/>
       <c r="AN45" t="inlineStr"/>
       <c r="AO45" t="inlineStr"/>
+      <c r="AP45" t="n">
+        <v>0.4932015496197691</v>
+      </c>
+      <c r="AQ45" t="n">
+        <v>0.6407102421388134</v>
+      </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
@@ -5934,6 +6208,12 @@
       <c r="AM46" t="inlineStr"/>
       <c r="AN46" t="inlineStr"/>
       <c r="AO46" t="inlineStr"/>
+      <c r="AP46" t="n">
+        <v>0.3348712956551398</v>
+      </c>
+      <c r="AQ46" t="n">
+        <v>0.442093355408133</v>
+      </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
@@ -6053,6 +6333,12 @@
       <c r="AM47" t="inlineStr"/>
       <c r="AN47" t="inlineStr"/>
       <c r="AO47" t="inlineStr"/>
+      <c r="AP47" t="n">
+        <v>0.3322798341632556</v>
+      </c>
+      <c r="AQ47" t="n">
+        <v>0.4251123254950276</v>
+      </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
@@ -6176,6 +6462,12 @@
       <c r="AM48" t="inlineStr"/>
       <c r="AN48" t="inlineStr"/>
       <c r="AO48" t="inlineStr"/>
+      <c r="AP48" t="n">
+        <v>0.0510524740622506</v>
+      </c>
+      <c r="AQ48" t="n">
+        <v>0.05417203797023321</v>
+      </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
@@ -6299,6 +6591,12 @@
       <c r="AM49" t="inlineStr"/>
       <c r="AN49" t="inlineStr"/>
       <c r="AO49" t="inlineStr"/>
+      <c r="AP49" t="n">
+        <v>0.07339548418386592</v>
+      </c>
+      <c r="AQ49" t="n">
+        <v>0.1855177958811558</v>
+      </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
@@ -6445,6 +6743,12 @@
       </c>
       <c r="AO50" t="n">
         <v>0.275376350719419</v>
+      </c>
+      <c r="AP50" t="n">
+        <v>0.6741923432873583</v>
+      </c>
+      <c r="AQ50" t="n">
+        <v>0.6610180995380134</v>
       </c>
     </row>
     <row r="51">
@@ -6567,6 +6871,12 @@
       <c r="AM51" t="inlineStr"/>
       <c r="AN51" t="inlineStr"/>
       <c r="AO51" t="inlineStr"/>
+      <c r="AP51" t="n">
+        <v>0.5110153735153735</v>
+      </c>
+      <c r="AQ51" t="n">
+        <v>0.5635847860221387</v>
+      </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
@@ -6692,6 +7002,12 @@
       <c r="AM52" t="inlineStr"/>
       <c r="AN52" t="inlineStr"/>
       <c r="AO52" t="inlineStr"/>
+      <c r="AP52" t="n">
+        <v>0.3337515999380406</v>
+      </c>
+      <c r="AQ52" t="n">
+        <v>0.477007938170499</v>
+      </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
@@ -6825,6 +7141,12 @@
       <c r="AM53" t="inlineStr"/>
       <c r="AN53" t="inlineStr"/>
       <c r="AO53" t="inlineStr"/>
+      <c r="AP53" t="n">
+        <v>0.6530352045425983</v>
+      </c>
+      <c r="AQ53" t="n">
+        <v>0.7357605611888884</v>
+      </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
@@ -6946,6 +7268,12 @@
       <c r="AM54" t="inlineStr"/>
       <c r="AN54" t="inlineStr"/>
       <c r="AO54" t="inlineStr"/>
+      <c r="AP54" t="n">
+        <v>0.3161117493126086</v>
+      </c>
+      <c r="AQ54" t="n">
+        <v>0.421237534843673</v>
+      </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
@@ -7069,6 +7397,12 @@
       <c r="AM55" t="inlineStr"/>
       <c r="AN55" t="inlineStr"/>
       <c r="AO55" t="inlineStr"/>
+      <c r="AP55" t="n">
+        <v>0.2885719493694787</v>
+      </c>
+      <c r="AQ55" t="n">
+        <v>0.4399255419724973</v>
+      </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
@@ -7190,6 +7524,12 @@
       <c r="AM56" t="inlineStr"/>
       <c r="AN56" t="inlineStr"/>
       <c r="AO56" t="inlineStr"/>
+      <c r="AP56" t="n">
+        <v>0.2952778569054741</v>
+      </c>
+      <c r="AQ56" t="n">
+        <v>0.4233480831331722</v>
+      </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
@@ -7315,6 +7655,12 @@
       <c r="AM57" t="inlineStr"/>
       <c r="AN57" t="inlineStr"/>
       <c r="AO57" t="inlineStr"/>
+      <c r="AP57" t="n">
+        <v>0.2132085441944597</v>
+      </c>
+      <c r="AQ57" t="n">
+        <v>0.3776978289587499</v>
+      </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
@@ -7436,6 +7782,12 @@
       <c r="AM58" t="inlineStr"/>
       <c r="AN58" t="inlineStr"/>
       <c r="AO58" t="inlineStr"/>
+      <c r="AP58" t="n">
+        <v>0.3156888390892884</v>
+      </c>
+      <c r="AQ58" t="n">
+        <v>0.4614666754151583</v>
+      </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
@@ -7563,6 +7915,12 @@
       <c r="AM59" t="inlineStr"/>
       <c r="AN59" t="inlineStr"/>
       <c r="AO59" t="inlineStr"/>
+      <c r="AP59" t="n">
+        <v>0.6087802758355657</v>
+      </c>
+      <c r="AQ59" t="n">
+        <v>0.6462357437147352</v>
+      </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
@@ -7680,6 +8038,12 @@
       <c r="AM60" t="inlineStr"/>
       <c r="AN60" t="inlineStr"/>
       <c r="AO60" t="inlineStr"/>
+      <c r="AP60" t="n">
+        <v>0.4978754157322784</v>
+      </c>
+      <c r="AQ60" t="n">
+        <v>0.6426532729796064</v>
+      </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
@@ -7789,6 +8153,12 @@
       <c r="AM61" t="inlineStr"/>
       <c r="AN61" t="inlineStr"/>
       <c r="AO61" t="inlineStr"/>
+      <c r="AP61" t="n">
+        <v>0.3186148701655053</v>
+      </c>
+      <c r="AQ61" t="n">
+        <v>0.4081245271460989</v>
+      </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
@@ -7902,6 +8272,12 @@
       <c r="AM62" t="inlineStr"/>
       <c r="AN62" t="inlineStr"/>
       <c r="AO62" t="inlineStr"/>
+      <c r="AP62" t="n">
+        <v>0.1479676096797846</v>
+      </c>
+      <c r="AQ62" t="n">
+        <v>0.2659569600042544</v>
+      </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
@@ -8025,6 +8401,12 @@
       <c r="AM63" t="inlineStr"/>
       <c r="AN63" t="inlineStr"/>
       <c r="AO63" t="inlineStr"/>
+      <c r="AP63" t="n">
+        <v>0.2360547553030816</v>
+      </c>
+      <c r="AQ63" t="n">
+        <v>0.3364908240406489</v>
+      </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
@@ -8146,6 +8528,12 @@
       <c r="AM64" t="inlineStr"/>
       <c r="AN64" t="inlineStr"/>
       <c r="AO64" t="inlineStr"/>
+      <c r="AP64" t="n">
+        <v>0.2469498055236595</v>
+      </c>
+      <c r="AQ64" t="n">
+        <v>0.3448875958069527</v>
+      </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
@@ -8267,6 +8655,12 @@
       <c r="AM65" t="inlineStr"/>
       <c r="AN65" t="inlineStr"/>
       <c r="AO65" t="inlineStr"/>
+      <c r="AP65" t="n">
+        <v>0.1328152134603748</v>
+      </c>
+      <c r="AQ65" t="n">
+        <v>0.6583508988879831</v>
+      </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
@@ -8388,6 +8782,12 @@
       <c r="AM66" t="inlineStr"/>
       <c r="AN66" t="inlineStr"/>
       <c r="AO66" t="inlineStr"/>
+      <c r="AP66" t="n">
+        <v>0.4145967884108302</v>
+      </c>
+      <c r="AQ66" t="n">
+        <v>0.5533410333830501</v>
+      </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
@@ -8517,6 +8917,12 @@
       <c r="AM67" t="inlineStr"/>
       <c r="AN67" t="inlineStr"/>
       <c r="AO67" t="inlineStr"/>
+      <c r="AP67" t="n">
+        <v>0.5881449364705272</v>
+      </c>
+      <c r="AQ67" t="n">
+        <v>0.6865318845580168</v>
+      </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
@@ -8640,6 +9046,12 @@
       <c r="AM68" t="inlineStr"/>
       <c r="AN68" t="inlineStr"/>
       <c r="AO68" t="inlineStr"/>
+      <c r="AP68" t="n">
+        <v>0.3734809314736526</v>
+      </c>
+      <c r="AQ68" t="n">
+        <v>0.5807089143928091</v>
+      </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
@@ -8763,6 +9175,12 @@
       <c r="AM69" t="inlineStr"/>
       <c r="AN69" t="inlineStr"/>
       <c r="AO69" t="inlineStr"/>
+      <c r="AP69" t="n">
+        <v>0.2975370226601753</v>
+      </c>
+      <c r="AQ69" t="n">
+        <v>0.4335351607753516</v>
+      </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
@@ -8886,6 +9304,12 @@
       <c r="AM70" t="inlineStr"/>
       <c r="AN70" t="inlineStr"/>
       <c r="AO70" t="inlineStr"/>
+      <c r="AP70" t="n">
+        <v>0.05805663870179999</v>
+      </c>
+      <c r="AQ70" t="n">
+        <v>0.1214436661878572</v>
+      </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
@@ -9023,6 +9447,12 @@
       <c r="AM71" t="inlineStr"/>
       <c r="AN71" t="inlineStr"/>
       <c r="AO71" t="inlineStr"/>
+      <c r="AP71" t="n">
+        <v>0.1275212206267204</v>
+      </c>
+      <c r="AQ71" t="n">
+        <v>0.6247631096631213</v>
+      </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
@@ -9134,6 +9564,12 @@
       <c r="AM72" t="inlineStr"/>
       <c r="AN72" t="inlineStr"/>
       <c r="AO72" t="inlineStr"/>
+      <c r="AP72" t="n">
+        <v>0.5349468894771923</v>
+      </c>
+      <c r="AQ72" t="n">
+        <v>0.6272622985163935</v>
+      </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
@@ -9255,6 +9691,12 @@
       <c r="AM73" t="inlineStr"/>
       <c r="AN73" t="inlineStr"/>
       <c r="AO73" t="inlineStr"/>
+      <c r="AP73" t="n">
+        <v>0.330404456574858</v>
+      </c>
+      <c r="AQ73" t="n">
+        <v>0.4841310050024503</v>
+      </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
@@ -9380,6 +9822,12 @@
       <c r="AM74" t="inlineStr"/>
       <c r="AN74" t="inlineStr"/>
       <c r="AO74" t="inlineStr"/>
+      <c r="AP74" t="n">
+        <v>0.2991220290293976</v>
+      </c>
+      <c r="AQ74" t="n">
+        <v>0.4295365149958162</v>
+      </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
@@ -9501,6 +9949,12 @@
       <c r="AM75" t="inlineStr"/>
       <c r="AN75" t="inlineStr"/>
       <c r="AO75" t="inlineStr"/>
+      <c r="AP75" t="n">
+        <v>0.0468384074941452</v>
+      </c>
+      <c r="AQ75" t="n">
+        <v>0.04703115814226926</v>
+      </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
@@ -9628,6 +10082,12 @@
       <c r="AM76" t="inlineStr"/>
       <c r="AN76" t="inlineStr"/>
       <c r="AO76" t="inlineStr"/>
+      <c r="AP76" t="n">
+        <v>0.4970158794079059</v>
+      </c>
+      <c r="AQ76" t="n">
+        <v>0.6750888985511115</v>
+      </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
@@ -9745,6 +10205,12 @@
       <c r="AM77" t="inlineStr"/>
       <c r="AN77" t="inlineStr"/>
       <c r="AO77" t="inlineStr"/>
+      <c r="AP77" t="n">
+        <v>0.3641294143076826</v>
+      </c>
+      <c r="AQ77" t="n">
+        <v>0.5502966630239673</v>
+      </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
@@ -9874,6 +10340,12 @@
       <c r="AM78" t="inlineStr"/>
       <c r="AN78" t="inlineStr"/>
       <c r="AO78" t="inlineStr"/>
+      <c r="AP78" t="n">
+        <v>0.6555122787425061</v>
+      </c>
+      <c r="AQ78" t="n">
+        <v>0.659894546142908</v>
+      </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
@@ -9995,6 +10467,12 @@
       <c r="AM79" t="inlineStr"/>
       <c r="AN79" t="inlineStr"/>
       <c r="AO79" t="inlineStr"/>
+      <c r="AP79" t="n">
+        <v>0.255240281941285</v>
+      </c>
+      <c r="AQ79" t="n">
+        <v>0.3131643820626199</v>
+      </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
@@ -10118,6 +10596,12 @@
       <c r="AM80" t="inlineStr"/>
       <c r="AN80" t="inlineStr"/>
       <c r="AO80" t="inlineStr"/>
+      <c r="AP80" t="n">
+        <v>0.1090158650387315</v>
+      </c>
+      <c r="AQ80" t="n">
+        <v>0.616146049169555</v>
+      </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
@@ -10241,6 +10725,12 @@
       <c r="AM81" t="inlineStr"/>
       <c r="AN81" t="inlineStr"/>
       <c r="AO81" t="inlineStr"/>
+      <c r="AP81" t="n">
+        <v>0.4996922359540862</v>
+      </c>
+      <c r="AQ81" t="n">
+        <v>0.6882347833531212</v>
+      </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
@@ -10366,6 +10856,12 @@
       <c r="AM82" t="inlineStr"/>
       <c r="AN82" t="inlineStr"/>
       <c r="AO82" t="inlineStr"/>
+      <c r="AP82" t="n">
+        <v>0.4788258953439843</v>
+      </c>
+      <c r="AQ82" t="n">
+        <v>0.570780091497434</v>
+      </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
@@ -10485,6 +10981,12 @@
       <c r="AM83" t="inlineStr"/>
       <c r="AN83" t="inlineStr"/>
       <c r="AO83" t="inlineStr"/>
+      <c r="AP83" t="n">
+        <v>0.1294422233327781</v>
+      </c>
+      <c r="AQ83" t="n">
+        <v>0.1541105331021297</v>
+      </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
@@ -10604,6 +11106,12 @@
       <c r="AM84" t="inlineStr"/>
       <c r="AN84" t="inlineStr"/>
       <c r="AO84" t="inlineStr"/>
+      <c r="AP84" t="n">
+        <v>0.2087871707822914</v>
+      </c>
+      <c r="AQ84" t="n">
+        <v>0.3873218653433051</v>
+      </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
@@ -10721,6 +11229,12 @@
       <c r="AM85" t="inlineStr"/>
       <c r="AN85" t="inlineStr"/>
       <c r="AO85" t="inlineStr"/>
+      <c r="AP85" t="n">
+        <v>0.3616484914063606</v>
+      </c>
+      <c r="AQ85" t="n">
+        <v>0.4687572305668721</v>
+      </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
@@ -10848,6 +11362,12 @@
       <c r="AM86" t="inlineStr"/>
       <c r="AN86" t="inlineStr"/>
       <c r="AO86" t="inlineStr"/>
+      <c r="AP86" t="n">
+        <v>0.5065892567267956</v>
+      </c>
+      <c r="AQ86" t="n">
+        <v>0.7258388047493892</v>
+      </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
@@ -10971,6 +11491,12 @@
       <c r="AM87" t="inlineStr"/>
       <c r="AN87" t="inlineStr"/>
       <c r="AO87" t="inlineStr"/>
+      <c r="AP87" t="n">
+        <v>0.2258343384428477</v>
+      </c>
+      <c r="AQ87" t="n">
+        <v>0.4402937156325524</v>
+      </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
@@ -11094,6 +11620,12 @@
       <c r="AM88" t="inlineStr"/>
       <c r="AN88" t="inlineStr"/>
       <c r="AO88" t="inlineStr"/>
+      <c r="AP88" t="n">
+        <v>0.252823479596935</v>
+      </c>
+      <c r="AQ88" t="n">
+        <v>0.5015772737575291</v>
+      </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
@@ -11215,6 +11747,12 @@
       <c r="AM89" t="inlineStr"/>
       <c r="AN89" t="inlineStr"/>
       <c r="AO89" t="inlineStr"/>
+      <c r="AP89" t="n">
+        <v>0.08814179148327142</v>
+      </c>
+      <c r="AQ89" t="n">
+        <v>0.1219104139351924</v>
+      </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
@@ -11336,6 +11874,12 @@
       <c r="AM90" t="inlineStr"/>
       <c r="AN90" t="inlineStr"/>
       <c r="AO90" t="inlineStr"/>
+      <c r="AP90" t="n">
+        <v>0.07062825130052021</v>
+      </c>
+      <c r="AQ90" t="n">
+        <v>0.17682394595265</v>
+      </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
@@ -11445,6 +11989,12 @@
       <c r="AM91" t="inlineStr"/>
       <c r="AN91" t="inlineStr"/>
       <c r="AO91" t="inlineStr"/>
+      <c r="AP91" t="n">
+        <v>0.0676270590606021</v>
+      </c>
+      <c r="AQ91" t="n">
+        <v>0.1879673726414063</v>
+      </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
@@ -11558,6 +12108,12 @@
       <c r="AM92" t="inlineStr"/>
       <c r="AN92" t="inlineStr"/>
       <c r="AO92" t="inlineStr"/>
+      <c r="AP92" t="n">
+        <v>0.4705866633220936</v>
+      </c>
+      <c r="AQ92" t="n">
+        <v>0.6020519940777497</v>
+      </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
@@ -11673,6 +12229,12 @@
       <c r="AM93" t="inlineStr"/>
       <c r="AN93" t="inlineStr"/>
       <c r="AO93" t="inlineStr"/>
+      <c r="AP93" t="n">
+        <v>0.0468384074941452</v>
+      </c>
+      <c r="AQ93" t="n">
+        <v>0.09924085576259488</v>
+      </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
@@ -11794,6 +12356,12 @@
       <c r="AM94" t="inlineStr"/>
       <c r="AN94" t="inlineStr"/>
       <c r="AO94" t="inlineStr"/>
+      <c r="AP94" t="n">
+        <v>0.1078361306298468</v>
+      </c>
+      <c r="AQ94" t="n">
+        <v>0.1334251793022408</v>
+      </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
@@ -11919,6 +12487,12 @@
       <c r="AM95" t="inlineStr"/>
       <c r="AN95" t="inlineStr"/>
       <c r="AO95" t="inlineStr"/>
+      <c r="AP95" t="n">
+        <v>0.1127685537491833</v>
+      </c>
+      <c r="AQ95" t="n">
+        <v>0.5510123710177425</v>
+      </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
@@ -12046,6 +12620,12 @@
       <c r="AM96" t="inlineStr"/>
       <c r="AN96" t="inlineStr"/>
       <c r="AO96" t="inlineStr"/>
+      <c r="AP96" t="n">
+        <v>0.4172087839120741</v>
+      </c>
+      <c r="AQ96" t="n">
+        <v>0.6445015204261908</v>
+      </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
@@ -12169,6 +12749,12 @@
       <c r="AM97" t="inlineStr"/>
       <c r="AN97" t="inlineStr"/>
       <c r="AO97" t="inlineStr"/>
+      <c r="AP97" t="n">
+        <v>0.05885093167701864</v>
+      </c>
+      <c r="AQ97" t="n">
+        <v>0.1576708527865616</v>
+      </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
@@ -12286,6 +12872,12 @@
       <c r="AM98" t="inlineStr"/>
       <c r="AN98" t="inlineStr"/>
       <c r="AO98" t="inlineStr"/>
+      <c r="AP98" t="n">
+        <v>0.3394920227397762</v>
+      </c>
+      <c r="AQ98" t="n">
+        <v>0.4405457927127269</v>
+      </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
@@ -12403,6 +12995,12 @@
       <c r="AM99" t="inlineStr"/>
       <c r="AN99" t="inlineStr"/>
       <c r="AO99" t="inlineStr"/>
+      <c r="AP99" t="n">
+        <v>0.3106274530423137</v>
+      </c>
+      <c r="AQ99" t="n">
+        <v>0.411223020729019</v>
+      </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
@@ -12514,6 +13112,12 @@
       <c r="AM100" t="inlineStr"/>
       <c r="AN100" t="inlineStr"/>
       <c r="AO100" t="inlineStr"/>
+      <c r="AP100" t="n">
+        <v>0.07977799056637232</v>
+      </c>
+      <c r="AQ100" t="n">
+        <v>0.08381522848637349</v>
+      </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
@@ -12627,6 +13231,12 @@
       <c r="AM101" t="inlineStr"/>
       <c r="AN101" t="inlineStr"/>
       <c r="AO101" t="inlineStr"/>
+      <c r="AP101" t="n">
+        <v>0.08702791461412152</v>
+      </c>
+      <c r="AQ101" t="n">
+        <v>0.4708214424499396</v>
+      </c>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
@@ -12750,6 +13360,12 @@
       <c r="AM102" t="inlineStr"/>
       <c r="AN102" t="inlineStr"/>
       <c r="AO102" t="inlineStr"/>
+      <c r="AP102" t="n">
+        <v>0.3976396812633746</v>
+      </c>
+      <c r="AQ102" t="n">
+        <v>0.5668278428236516</v>
+      </c>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
@@ -12873,6 +13489,12 @@
       <c r="AM103" t="inlineStr"/>
       <c r="AN103" t="inlineStr"/>
       <c r="AO103" t="inlineStr"/>
+      <c r="AP103" t="n">
+        <v>0.1396715820434802</v>
+      </c>
+      <c r="AQ103" t="n">
+        <v>0.3377273898908263</v>
+      </c>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
@@ -12994,6 +13616,12 @@
       <c r="AM104" t="inlineStr"/>
       <c r="AN104" t="inlineStr"/>
       <c r="AO104" t="inlineStr"/>
+      <c r="AP104" t="n">
+        <v>0.02197802197802198</v>
+      </c>
+      <c r="AQ104" t="n">
+        <v>0.06772486772486772</v>
+      </c>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
@@ -13103,6 +13731,12 @@
       <c r="AM105" t="inlineStr"/>
       <c r="AN105" t="inlineStr"/>
       <c r="AO105" t="inlineStr"/>
+      <c r="AP105" t="n">
+        <v>0.5164266143615077</v>
+      </c>
+      <c r="AQ105" t="n">
+        <v>0.6484286546019039</v>
+      </c>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
@@ -13226,6 +13860,12 @@
       <c r="AM106" t="inlineStr"/>
       <c r="AN106" t="inlineStr"/>
       <c r="AO106" t="inlineStr"/>
+      <c r="AP106" t="n">
+        <v>0.0925170068027211</v>
+      </c>
+      <c r="AQ106" t="n">
+        <v>0.5857346221184476</v>
+      </c>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
@@ -13353,6 +13993,12 @@
       <c r="AM107" t="inlineStr"/>
       <c r="AN107" t="inlineStr"/>
       <c r="AO107" t="inlineStr"/>
+      <c r="AP107" t="n">
+        <v>0.4968088568426841</v>
+      </c>
+      <c r="AQ107" t="n">
+        <v>0.7017453084481895</v>
+      </c>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
@@ -13476,6 +14122,12 @@
       <c r="AM108" t="inlineStr"/>
       <c r="AN108" t="inlineStr"/>
       <c r="AO108" t="inlineStr"/>
+      <c r="AP108" t="n">
+        <v>0.3220333746259771</v>
+      </c>
+      <c r="AQ108" t="n">
+        <v>0.427758713470153</v>
+      </c>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
@@ -13587,6 +14239,12 @@
       <c r="AM109" t="inlineStr"/>
       <c r="AN109" t="inlineStr"/>
       <c r="AO109" t="inlineStr"/>
+      <c r="AP109" t="n">
+        <v>0.101512871776903</v>
+      </c>
+      <c r="AQ109" t="n">
+        <v>0.579481933420418</v>
+      </c>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr">
@@ -13696,6 +14354,12 @@
       <c r="AM110" t="inlineStr"/>
       <c r="AN110" t="inlineStr"/>
       <c r="AO110" t="inlineStr"/>
+      <c r="AP110" t="n">
+        <v>0.2668122691599052</v>
+      </c>
+      <c r="AQ110" t="n">
+        <v>0.4755326354272157</v>
+      </c>
     </row>
     <row r="111">
       <c r="A111" t="inlineStr">
@@ -13817,6 +14481,12 @@
       <c r="AM111" t="inlineStr"/>
       <c r="AN111" t="inlineStr"/>
       <c r="AO111" t="inlineStr"/>
+      <c r="AP111" t="n">
+        <v>0.3846356011609571</v>
+      </c>
+      <c r="AQ111" t="n">
+        <v>0.5724506038010595</v>
+      </c>
     </row>
     <row r="112">
       <c r="A112" t="inlineStr">
@@ -13938,6 +14608,12 @@
       <c r="AM112" t="inlineStr"/>
       <c r="AN112" t="inlineStr"/>
       <c r="AO112" t="inlineStr"/>
+      <c r="AP112" t="n">
+        <v>0.3932958813256376</v>
+      </c>
+      <c r="AQ112" t="n">
+        <v>0.5415725578769057</v>
+      </c>
     </row>
     <row r="113">
       <c r="A113" t="inlineStr">
@@ -14065,6 +14741,12 @@
       <c r="AM113" t="inlineStr"/>
       <c r="AN113" t="inlineStr"/>
       <c r="AO113" t="inlineStr"/>
+      <c r="AP113" t="n">
+        <v>0.4016678470459983</v>
+      </c>
+      <c r="AQ113" t="n">
+        <v>0.6261498620070503</v>
+      </c>
     </row>
     <row r="114">
       <c r="A114" t="inlineStr">
@@ -14184,6 +14866,12 @@
       <c r="AM114" t="inlineStr"/>
       <c r="AN114" t="inlineStr"/>
       <c r="AO114" t="inlineStr"/>
+      <c r="AP114" t="n">
+        <v>0.3692735224351149</v>
+      </c>
+      <c r="AQ114" t="n">
+        <v>0.4812736910733079</v>
+      </c>
     </row>
     <row r="115">
       <c r="A115" t="inlineStr">
@@ -14301,6 +14989,12 @@
       <c r="AM115" t="inlineStr"/>
       <c r="AN115" t="inlineStr"/>
       <c r="AO115" t="inlineStr"/>
+      <c r="AP115" t="n">
+        <v>0.3953191552365239</v>
+      </c>
+      <c r="AQ115" t="n">
+        <v>0.5799649729245936</v>
+      </c>
     </row>
     <row r="116">
       <c r="A116" t="inlineStr">
@@ -14414,6 +15108,12 @@
       <c r="AM116" t="inlineStr"/>
       <c r="AN116" t="inlineStr"/>
       <c r="AO116" t="inlineStr"/>
+      <c r="AP116" t="n">
+        <v>0.07407998486836662</v>
+      </c>
+      <c r="AQ116" t="n">
+        <v>0.4854740911262651</v>
+      </c>
     </row>
     <row r="117">
       <c r="A117" t="inlineStr">
@@ -14533,6 +15233,12 @@
       <c r="AM117" t="inlineStr"/>
       <c r="AN117" t="inlineStr"/>
       <c r="AO117" t="inlineStr"/>
+      <c r="AP117" t="n">
+        <v>0.5794045423760306</v>
+      </c>
+      <c r="AQ117" t="n">
+        <v>0.6736265124851949</v>
+      </c>
     </row>
     <row r="118">
       <c r="A118" t="inlineStr">
@@ -14650,6 +15356,12 @@
       <c r="AM118" t="inlineStr"/>
       <c r="AN118" t="inlineStr"/>
       <c r="AO118" t="inlineStr"/>
+      <c r="AP118" t="n">
+        <v>0.5729742939506899</v>
+      </c>
+      <c r="AQ118" t="n">
+        <v>0.6935374301055043</v>
+      </c>
     </row>
     <row r="119">
       <c r="A119" t="inlineStr">
@@ -14775,6 +15487,12 @@
       <c r="AM119" t="inlineStr"/>
       <c r="AN119" t="inlineStr"/>
       <c r="AO119" t="inlineStr"/>
+      <c r="AP119" t="n">
+        <v>0.5742580548702998</v>
+      </c>
+      <c r="AQ119" t="n">
+        <v>0.7433424389316764</v>
+      </c>
     </row>
     <row r="120">
       <c r="A120" t="inlineStr">
@@ -14900,6 +15618,12 @@
       <c r="AM120" t="inlineStr"/>
       <c r="AN120" t="inlineStr"/>
       <c r="AO120" t="inlineStr"/>
+      <c r="AP120" t="n">
+        <v>0.5632560201649133</v>
+      </c>
+      <c r="AQ120" t="n">
+        <v>0.7055029519315233</v>
+      </c>
     </row>
     <row r="121">
       <c r="A121" t="inlineStr">
@@ -15017,6 +15741,12 @@
       <c r="AM121" t="inlineStr"/>
       <c r="AN121" t="inlineStr"/>
       <c r="AO121" t="inlineStr"/>
+      <c r="AP121" t="n">
+        <v>0.0468384074941452</v>
+      </c>
+      <c r="AQ121" t="n">
+        <v>0.07233124018838304</v>
+      </c>
     </row>
     <row r="122">
       <c r="A122" t="inlineStr">
@@ -15138,6 +15868,12 @@
       <c r="AM122" t="inlineStr"/>
       <c r="AN122" t="inlineStr"/>
       <c r="AO122" t="inlineStr"/>
+      <c r="AP122" t="n">
+        <v>0.5030476340459323</v>
+      </c>
+      <c r="AQ122" t="n">
+        <v>0.6346833749281612</v>
+      </c>
     </row>
     <row r="123">
       <c r="A123" t="inlineStr">
@@ -15259,6 +15995,12 @@
       <c r="AM123" t="inlineStr"/>
       <c r="AN123" t="inlineStr"/>
       <c r="AO123" t="inlineStr"/>
+      <c r="AP123" t="n">
+        <v>0.1308535735677004</v>
+      </c>
+      <c r="AQ123" t="n">
+        <v>0.3969922692348057</v>
+      </c>
     </row>
     <row r="124">
       <c r="A124" t="inlineStr">
@@ -15380,6 +16122,12 @@
       <c r="AM124" t="inlineStr"/>
       <c r="AN124" t="inlineStr"/>
       <c r="AO124" t="inlineStr"/>
+      <c r="AP124" t="n">
+        <v>0.3299661572827648</v>
+      </c>
+      <c r="AQ124" t="n">
+        <v>0.5782244463672892</v>
+      </c>
     </row>
     <row r="125">
       <c r="A125" t="inlineStr">
@@ -15501,6 +16249,12 @@
       <c r="AM125" t="inlineStr"/>
       <c r="AN125" t="inlineStr"/>
       <c r="AO125" t="inlineStr"/>
+      <c r="AP125" t="n">
+        <v>0.1638731039350845</v>
+      </c>
+      <c r="AQ125" t="n">
+        <v>0.3175500210625337</v>
+      </c>
     </row>
     <row r="126">
       <c r="A126" t="inlineStr">
@@ -15618,6 +16372,12 @@
       <c r="AM126" t="inlineStr"/>
       <c r="AN126" t="inlineStr"/>
       <c r="AO126" t="inlineStr"/>
+      <c r="AP126" t="n">
+        <v>0.240424293055872</v>
+      </c>
+      <c r="AQ126" t="n">
+        <v>0.407833827370674</v>
+      </c>
     </row>
     <row r="127">
       <c r="A127" t="inlineStr">
@@ -15743,6 +16503,12 @@
       <c r="AM127" t="inlineStr"/>
       <c r="AN127" t="inlineStr"/>
       <c r="AO127" t="inlineStr"/>
+      <c r="AP127" t="n">
+        <v>0.2704651467703464</v>
+      </c>
+      <c r="AQ127" t="n">
+        <v>0.3746344602442163</v>
+      </c>
     </row>
     <row r="128">
       <c r="A128" t="inlineStr">
@@ -15866,6 +16632,12 @@
       <c r="AM128" t="inlineStr"/>
       <c r="AN128" t="inlineStr"/>
       <c r="AO128" t="inlineStr"/>
+      <c r="AP128" t="n">
+        <v>0.03034134007585335</v>
+      </c>
+      <c r="AQ128" t="n">
+        <v>0.07290725918176899</v>
+      </c>
     </row>
     <row r="129">
       <c r="A129" t="inlineStr">
@@ -15987,6 +16759,12 @@
       <c r="AM129" t="inlineStr"/>
       <c r="AN129" t="inlineStr"/>
       <c r="AO129" t="inlineStr"/>
+      <c r="AP129" t="n">
+        <v>0.4486106239268867</v>
+      </c>
+      <c r="AQ129" t="n">
+        <v>0.5890114227509187</v>
+      </c>
     </row>
     <row r="130">
       <c r="A130" t="inlineStr">
@@ -16108,6 +16886,12 @@
       <c r="AM130" t="inlineStr"/>
       <c r="AN130" t="inlineStr"/>
       <c r="AO130" t="inlineStr"/>
+      <c r="AP130" t="n">
+        <v>0.07803370310779914</v>
+      </c>
+      <c r="AQ130" t="n">
+        <v>0.6211648845711774</v>
+      </c>
     </row>
     <row r="131">
       <c r="A131" t="inlineStr">
@@ -16231,6 +17015,12 @@
       <c r="AM131" t="inlineStr"/>
       <c r="AN131" t="inlineStr"/>
       <c r="AO131" t="inlineStr"/>
+      <c r="AP131" t="n">
+        <v>0.4572353422324961</v>
+      </c>
+      <c r="AQ131" t="n">
+        <v>0.5647660893379266</v>
+      </c>
     </row>
     <row r="132">
       <c r="A132" t="inlineStr">
@@ -16358,6 +17148,12 @@
       <c r="AM132" t="inlineStr"/>
       <c r="AN132" t="inlineStr"/>
       <c r="AO132" t="inlineStr"/>
+      <c r="AP132" t="n">
+        <v>0.1292414959294755</v>
+      </c>
+      <c r="AQ132" t="n">
+        <v>0.6745996674752559</v>
+      </c>
     </row>
     <row r="133">
       <c r="A133" t="inlineStr">
@@ -16479,6 +17275,12 @@
       <c r="AM133" t="inlineStr"/>
       <c r="AN133" t="inlineStr"/>
       <c r="AO133" t="inlineStr"/>
+      <c r="AP133" t="n">
+        <v>0.4685674070767239</v>
+      </c>
+      <c r="AQ133" t="n">
+        <v>0.5988106594066431</v>
+      </c>
     </row>
     <row r="134">
       <c r="A134" t="inlineStr">
@@ -16590,6 +17392,12 @@
       <c r="AM134" t="inlineStr"/>
       <c r="AN134" t="inlineStr"/>
       <c r="AO134" t="inlineStr"/>
+      <c r="AP134" t="n">
+        <v>0.1095494889788448</v>
+      </c>
+      <c r="AQ134" t="n">
+        <v>0.223769620524266</v>
+      </c>
     </row>
     <row r="135">
       <c r="A135" t="inlineStr">
@@ -16715,6 +17523,12 @@
       <c r="AM135" t="inlineStr"/>
       <c r="AN135" t="inlineStr"/>
       <c r="AO135" t="inlineStr"/>
+      <c r="AP135" t="n">
+        <v>0.4804195899470956</v>
+      </c>
+      <c r="AQ135" t="n">
+        <v>0.6644827113884471</v>
+      </c>
     </row>
     <row r="136">
       <c r="A136" t="inlineStr">
@@ -16836,6 +17650,12 @@
       <c r="AM136" t="inlineStr"/>
       <c r="AN136" t="inlineStr"/>
       <c r="AO136" t="inlineStr"/>
+      <c r="AP136" t="n">
+        <v>0.6062809326178361</v>
+      </c>
+      <c r="AQ136" t="n">
+        <v>0.6574965987681505</v>
+      </c>
     </row>
     <row r="137">
       <c r="A137" t="inlineStr">
@@ -16955,6 +17775,12 @@
       <c r="AM137" t="inlineStr"/>
       <c r="AN137" t="inlineStr"/>
       <c r="AO137" t="inlineStr"/>
+      <c r="AP137" t="n">
+        <v>0.6461005949978446</v>
+      </c>
+      <c r="AQ137" t="n">
+        <v>0.6876607440911406</v>
+      </c>
     </row>
     <row r="138">
       <c r="A138" t="inlineStr">
@@ -17074,6 +17900,12 @@
       <c r="AM138" t="inlineStr"/>
       <c r="AN138" t="inlineStr"/>
       <c r="AO138" t="inlineStr"/>
+      <c r="AP138" t="n">
+        <v>0.5190850286368428</v>
+      </c>
+      <c r="AQ138" t="n">
+        <v>0.5885499069444344</v>
+      </c>
     </row>
     <row r="139">
       <c r="A139" t="inlineStr">
@@ -17201,6 +18033,12 @@
       <c r="AM139" t="inlineStr"/>
       <c r="AN139" t="inlineStr"/>
       <c r="AO139" t="inlineStr"/>
+      <c r="AP139" t="n">
+        <v>0.5470928372179085</v>
+      </c>
+      <c r="AQ139" t="n">
+        <v>0.7057166063949715</v>
+      </c>
     </row>
     <row r="140">
       <c r="A140" t="inlineStr">
@@ -17320,6 +18158,12 @@
       <c r="AM140" t="inlineStr"/>
       <c r="AN140" t="inlineStr"/>
       <c r="AO140" t="inlineStr"/>
+      <c r="AP140" t="n">
+        <v>0.428036765744407</v>
+      </c>
+      <c r="AQ140" t="n">
+        <v>0.6207281144781145</v>
+      </c>
     </row>
     <row r="141">
       <c r="A141" t="inlineStr">
@@ -17433,6 +18277,12 @@
       <c r="AM141" t="inlineStr"/>
       <c r="AN141" t="inlineStr"/>
       <c r="AO141" t="inlineStr"/>
+      <c r="AP141" t="n">
+        <v>0.2002817288531575</v>
+      </c>
+      <c r="AQ141" t="n">
+        <v>0.4163384194866642</v>
+      </c>
     </row>
     <row r="142">
       <c r="A142" t="inlineStr">
@@ -17556,6 +18406,12 @@
       <c r="AM142" t="inlineStr"/>
       <c r="AN142" t="inlineStr"/>
       <c r="AO142" t="inlineStr"/>
+      <c r="AP142" t="n">
+        <v>0.2619199437936812</v>
+      </c>
+      <c r="AQ142" t="n">
+        <v>0.5409426780116434</v>
+      </c>
     </row>
     <row r="143">
       <c r="A143" t="inlineStr">
@@ -17665,6 +18521,12 @@
       <c r="AM143" t="inlineStr"/>
       <c r="AN143" t="inlineStr"/>
       <c r="AO143" t="inlineStr"/>
+      <c r="AP143" t="n">
+        <v>0.3160992783934283</v>
+      </c>
+      <c r="AQ143" t="n">
+        <v>0.4451210525445353</v>
+      </c>
     </row>
     <row r="144">
       <c r="A144" t="inlineStr">
@@ -17786,6 +18648,12 @@
       <c r="AM144" t="inlineStr"/>
       <c r="AN144" t="inlineStr"/>
       <c r="AO144" t="inlineStr"/>
+      <c r="AP144" t="n">
+        <v>0.3596678610586804</v>
+      </c>
+      <c r="AQ144" t="n">
+        <v>0.5346053725588676</v>
+      </c>
     </row>
     <row r="145">
       <c r="A145" t="inlineStr">
@@ -17913,6 +18781,12 @@
       <c r="AM145" t="inlineStr"/>
       <c r="AN145" t="inlineStr"/>
       <c r="AO145" t="inlineStr"/>
+      <c r="AP145" t="n">
+        <v>0.6551947351386341</v>
+      </c>
+      <c r="AQ145" t="n">
+        <v>0.6296424091573007</v>
+      </c>
     </row>
     <row r="146">
       <c r="A146" t="inlineStr">
@@ -18022,6 +18896,12 @@
       <c r="AM146" t="inlineStr"/>
       <c r="AN146" t="inlineStr"/>
       <c r="AO146" t="inlineStr"/>
+      <c r="AP146" t="n">
+        <v>0.248015001154528</v>
+      </c>
+      <c r="AQ146" t="n">
+        <v>0.5741343526220577</v>
+      </c>
     </row>
     <row r="147">
       <c r="A147" t="inlineStr">
@@ -18135,6 +19015,12 @@
       <c r="AM147" t="inlineStr"/>
       <c r="AN147" t="inlineStr"/>
       <c r="AO147" t="inlineStr"/>
+      <c r="AP147" t="n">
+        <v>0.3816019936863028</v>
+      </c>
+      <c r="AQ147" t="n">
+        <v>0.4686373038836901</v>
+      </c>
     </row>
     <row r="148">
       <c r="A148" t="inlineStr">
@@ -18256,6 +19142,12 @@
       <c r="AM148" t="inlineStr"/>
       <c r="AN148" t="inlineStr"/>
       <c r="AO148" t="inlineStr"/>
+      <c r="AP148" t="n">
+        <v>0.4615816146583976</v>
+      </c>
+      <c r="AQ148" t="n">
+        <v>0.5888324206578032</v>
+      </c>
     </row>
     <row r="149">
       <c r="A149" t="inlineStr">
@@ -18381,6 +19273,12 @@
       <c r="AM149" t="inlineStr"/>
       <c r="AN149" t="inlineStr"/>
       <c r="AO149" t="inlineStr"/>
+      <c r="AP149" t="n">
+        <v>0.4681782796337025</v>
+      </c>
+      <c r="AQ149" t="n">
+        <v>0.662102359527081</v>
+      </c>
     </row>
     <row r="150">
       <c r="A150" t="inlineStr">
@@ -18504,6 +19402,12 @@
       <c r="AM150" t="inlineStr"/>
       <c r="AN150" t="inlineStr"/>
       <c r="AO150" t="inlineStr"/>
+      <c r="AP150" t="n">
+        <v>0.1883303539444593</v>
+      </c>
+      <c r="AQ150" t="n">
+        <v>0.5371886567538742</v>
+      </c>
     </row>
     <row r="151">
       <c r="A151" t="inlineStr">
@@ -18627,6 +19531,12 @@
       <c r="AM151" t="inlineStr"/>
       <c r="AN151" t="inlineStr"/>
       <c r="AO151" t="inlineStr"/>
+      <c r="AP151" t="n">
+        <v>0.2975777881774179</v>
+      </c>
+      <c r="AQ151" t="n">
+        <v>0.4425290537372008</v>
+      </c>
     </row>
     <row r="152">
       <c r="A152" t="inlineStr">
@@ -18748,6 +19658,12 @@
       <c r="AM152" t="inlineStr"/>
       <c r="AN152" t="inlineStr"/>
       <c r="AO152" t="inlineStr"/>
+      <c r="AP152" t="n">
+        <v>0.4641323044293663</v>
+      </c>
+      <c r="AQ152" t="n">
+        <v>0.686750547213421</v>
+      </c>
     </row>
     <row r="153">
       <c r="A153" t="inlineStr">
@@ -18865,6 +19781,12 @@
       <c r="AM153" t="inlineStr"/>
       <c r="AN153" t="inlineStr"/>
       <c r="AO153" t="inlineStr"/>
+      <c r="AP153" t="n">
+        <v>0.02445302445302445</v>
+      </c>
+      <c r="AQ153" t="n">
+        <v>0.06835776440325418</v>
+      </c>
     </row>
     <row r="154">
       <c r="A154" t="inlineStr">
@@ -18982,6 +19904,12 @@
       <c r="AM154" t="inlineStr"/>
       <c r="AN154" t="inlineStr"/>
       <c r="AO154" t="inlineStr"/>
+      <c r="AP154" t="n">
+        <v>0.4245526087091981</v>
+      </c>
+      <c r="AQ154" t="n">
+        <v>0.5838053601001343</v>
+      </c>
     </row>
     <row r="155">
       <c r="A155" t="inlineStr">
@@ -19101,6 +20029,12 @@
       <c r="AM155" t="inlineStr"/>
       <c r="AN155" t="inlineStr"/>
       <c r="AO155" t="inlineStr"/>
+      <c r="AP155" t="n">
+        <v>0.05096937458514639</v>
+      </c>
+      <c r="AQ155" t="n">
+        <v>0.04304531473059885</v>
+      </c>
     </row>
     <row r="156">
       <c r="A156" t="inlineStr">
@@ -19224,6 +20158,12 @@
       <c r="AM156" t="inlineStr"/>
       <c r="AN156" t="inlineStr"/>
       <c r="AO156" t="inlineStr"/>
+      <c r="AP156" t="n">
+        <v>0.0303030303030303</v>
+      </c>
+      <c r="AQ156" t="n">
+        <v>0.06403745212086821</v>
+      </c>
     </row>
     <row r="157">
       <c r="A157" t="inlineStr">
@@ -19345,6 +20285,12 @@
       <c r="AM157" t="inlineStr"/>
       <c r="AN157" t="inlineStr"/>
       <c r="AO157" t="inlineStr"/>
+      <c r="AP157" t="n">
+        <v>0.3451290300644677</v>
+      </c>
+      <c r="AQ157" t="n">
+        <v>0.5141063649609015</v>
+      </c>
     </row>
     <row r="158">
       <c r="A158" t="inlineStr">
@@ -19466,6 +20412,12 @@
       <c r="AM158" t="inlineStr"/>
       <c r="AN158" t="inlineStr"/>
       <c r="AO158" t="inlineStr"/>
+      <c r="AP158" t="n">
+        <v>0.3777696312539519</v>
+      </c>
+      <c r="AQ158" t="n">
+        <v>0.5364208485326498</v>
+      </c>
     </row>
     <row r="159">
       <c r="A159" t="inlineStr">
@@ -19587,6 +20539,12 @@
       <c r="AM159" t="inlineStr"/>
       <c r="AN159" t="inlineStr"/>
       <c r="AO159" t="inlineStr"/>
+      <c r="AP159" t="n">
+        <v>0.2721808750261924</v>
+      </c>
+      <c r="AQ159" t="n">
+        <v>0.3821397990326848</v>
+      </c>
     </row>
     <row r="160">
       <c r="A160" t="inlineStr">
@@ -19712,6 +20670,12 @@
       <c r="AM160" t="inlineStr"/>
       <c r="AN160" t="inlineStr"/>
       <c r="AO160" t="inlineStr"/>
+      <c r="AP160" t="n">
+        <v>0.5060607826825697</v>
+      </c>
+      <c r="AQ160" t="n">
+        <v>0.5874929972868224</v>
+      </c>
     </row>
     <row r="161">
       <c r="A161" t="inlineStr">
@@ -19837,6 +20801,12 @@
       <c r="AM161" t="inlineStr"/>
       <c r="AN161" t="inlineStr"/>
       <c r="AO161" t="inlineStr"/>
+      <c r="AP161" t="n">
+        <v>0.1285646720429329</v>
+      </c>
+      <c r="AQ161" t="n">
+        <v>0.3413920232288229</v>
+      </c>
     </row>
     <row r="162">
       <c r="A162" t="inlineStr">
@@ -19958,6 +20928,12 @@
       <c r="AM162" t="inlineStr"/>
       <c r="AN162" t="inlineStr"/>
       <c r="AO162" t="inlineStr"/>
+      <c r="AP162" t="n">
+        <v>0.2260310390612274</v>
+      </c>
+      <c r="AQ162" t="n">
+        <v>0.349557416302147</v>
+      </c>
     </row>
     <row r="163">
       <c r="A163" t="inlineStr">
@@ -20087,6 +21063,12 @@
       <c r="AM163" t="inlineStr"/>
       <c r="AN163" t="inlineStr"/>
       <c r="AO163" t="inlineStr"/>
+      <c r="AP163" t="n">
+        <v>0.4602907502067166</v>
+      </c>
+      <c r="AQ163" t="n">
+        <v>0.5912817275706324</v>
+      </c>
     </row>
     <row r="164">
       <c r="A164" t="inlineStr">
@@ -20214,6 +21196,12 @@
       <c r="AM164" t="inlineStr"/>
       <c r="AN164" t="inlineStr"/>
       <c r="AO164" t="inlineStr"/>
+      <c r="AP164" t="n">
+        <v>0.6458694208133198</v>
+      </c>
+      <c r="AQ164" t="n">
+        <v>0.6543764005382566</v>
+      </c>
     </row>
     <row r="165">
       <c r="A165" t="inlineStr">
@@ -20335,6 +21323,12 @@
       <c r="AM165" t="inlineStr"/>
       <c r="AN165" t="inlineStr"/>
       <c r="AO165" t="inlineStr"/>
+      <c r="AP165" t="n">
+        <v>0.5511166466323064</v>
+      </c>
+      <c r="AQ165" t="n">
+        <v>0.6256248851541921</v>
+      </c>
     </row>
     <row r="166">
       <c r="A166" t="inlineStr">
@@ -20458,6 +21452,12 @@
       <c r="AM166" t="inlineStr"/>
       <c r="AN166" t="inlineStr"/>
       <c r="AO166" t="inlineStr"/>
+      <c r="AP166" t="n">
+        <v>0.1261672243004885</v>
+      </c>
+      <c r="AQ166" t="n">
+        <v>0.4085829195346439</v>
+      </c>
     </row>
     <row r="167">
       <c r="A167" t="inlineStr">
@@ -20581,6 +21581,12 @@
       <c r="AM167" t="inlineStr"/>
       <c r="AN167" t="inlineStr"/>
       <c r="AO167" t="inlineStr"/>
+      <c r="AP167" t="n">
+        <v>0.3736789388801772</v>
+      </c>
+      <c r="AQ167" t="n">
+        <v>0.5976567292356767</v>
+      </c>
     </row>
     <row r="168">
       <c r="A168" t="inlineStr">
@@ -20702,6 +21708,12 @@
       <c r="AM168" t="inlineStr"/>
       <c r="AN168" t="inlineStr"/>
       <c r="AO168" t="inlineStr"/>
+      <c r="AP168" t="n">
+        <v>0.4937869167957177</v>
+      </c>
+      <c r="AQ168" t="n">
+        <v>0.6360625221141392</v>
+      </c>
     </row>
     <row r="169">
       <c r="A169" t="inlineStr">
@@ -20823,6 +21835,12 @@
       <c r="AM169" t="inlineStr"/>
       <c r="AN169" t="inlineStr"/>
       <c r="AO169" t="inlineStr"/>
+      <c r="AP169" t="n">
+        <v>0.1105519633490234</v>
+      </c>
+      <c r="AQ169" t="n">
+        <v>0.5519770563359578</v>
+      </c>
     </row>
     <row r="170">
       <c r="A170" t="inlineStr">
@@ -20946,6 +21964,12 @@
       <c r="AM170" t="inlineStr"/>
       <c r="AN170" t="inlineStr"/>
       <c r="AO170" t="inlineStr"/>
+      <c r="AP170" t="n">
+        <v>0.4983301070257592</v>
+      </c>
+      <c r="AQ170" t="n">
+        <v>0.6691514846762463</v>
+      </c>
     </row>
     <row r="171">
       <c r="A171" t="inlineStr">
@@ -21055,6 +22079,12 @@
       <c r="AM171" t="inlineStr"/>
       <c r="AN171" t="inlineStr"/>
       <c r="AO171" t="inlineStr"/>
+      <c r="AP171" t="n">
+        <v>0.3350484676142571</v>
+      </c>
+      <c r="AQ171" t="n">
+        <v>0.5018961000549288</v>
+      </c>
     </row>
     <row r="172">
       <c r="A172" t="inlineStr">
@@ -21182,6 +22212,12 @@
       <c r="AM172" t="inlineStr"/>
       <c r="AN172" t="inlineStr"/>
       <c r="AO172" t="inlineStr"/>
+      <c r="AP172" t="n">
+        <v>0.1416064222515835</v>
+      </c>
+      <c r="AQ172" t="n">
+        <v>0.6747498609899044</v>
+      </c>
     </row>
     <row r="173">
       <c r="A173" t="inlineStr">
@@ -21291,6 +22327,12 @@
       <c r="AM173" t="inlineStr"/>
       <c r="AN173" t="inlineStr"/>
       <c r="AO173" t="inlineStr"/>
+      <c r="AP173" t="n">
+        <v>0.2587894016465445</v>
+      </c>
+      <c r="AQ173" t="n">
+        <v>0.3971439119886325</v>
+      </c>
     </row>
     <row r="174">
       <c r="A174" t="inlineStr">
@@ -21400,6 +22442,12 @@
       <c r="AM174" t="inlineStr"/>
       <c r="AN174" t="inlineStr"/>
       <c r="AO174" t="inlineStr"/>
+      <c r="AP174" t="n">
+        <v>0.03300756922487304</v>
+      </c>
+      <c r="AQ174" t="n">
+        <v>0.09109105180533751</v>
+      </c>
     </row>
     <row r="175">
       <c r="A175" t="inlineStr">
@@ -21521,6 +22569,12 @@
       <c r="AM175" t="inlineStr"/>
       <c r="AN175" t="inlineStr"/>
       <c r="AO175" t="inlineStr"/>
+      <c r="AP175" t="n">
+        <v>0.06040847119685295</v>
+      </c>
+      <c r="AQ175" t="n">
+        <v>0.1495090171955633</v>
+      </c>
     </row>
     <row r="176">
       <c r="A176" t="inlineStr">
@@ -21648,6 +22702,12 @@
       <c r="AM176" t="inlineStr"/>
       <c r="AN176" t="inlineStr"/>
       <c r="AO176" t="inlineStr"/>
+      <c r="AP176" t="n">
+        <v>0.5335469695124427</v>
+      </c>
+      <c r="AQ176" t="n">
+        <v>0.7591339785080562</v>
+      </c>
     </row>
     <row r="177">
       <c r="A177" t="inlineStr">
@@ -21771,6 +22831,12 @@
       <c r="AM177" t="inlineStr"/>
       <c r="AN177" t="inlineStr"/>
       <c r="AO177" t="inlineStr"/>
+      <c r="AP177" t="n">
+        <v>0.0468384074941452</v>
+      </c>
+      <c r="AQ177" t="n">
+        <v>0.1303958307888912</v>
+      </c>
     </row>
     <row r="178">
       <c r="A178" t="inlineStr">
@@ -21892,6 +22958,12 @@
       <c r="AM178" t="inlineStr"/>
       <c r="AN178" t="inlineStr"/>
       <c r="AO178" t="inlineStr"/>
+      <c r="AP178" t="n">
+        <v>0.3761963212950797</v>
+      </c>
+      <c r="AQ178" t="n">
+        <v>0.586338757327618</v>
+      </c>
     </row>
     <row r="179">
       <c r="A179" t="inlineStr">
@@ -22015,6 +23087,12 @@
       <c r="AM179" t="inlineStr"/>
       <c r="AN179" t="inlineStr"/>
       <c r="AO179" t="inlineStr"/>
+      <c r="AP179" t="n">
+        <v>0.05576533109572758</v>
+      </c>
+      <c r="AQ179" t="n">
+        <v>0.09740007113956693</v>
+      </c>
     </row>
     <row r="180">
       <c r="A180" t="inlineStr">
@@ -22138,6 +23216,12 @@
       <c r="AM180" t="inlineStr"/>
       <c r="AN180" t="inlineStr"/>
       <c r="AO180" t="inlineStr"/>
+      <c r="AP180" t="n">
+        <v>0.05644381646463896</v>
+      </c>
+      <c r="AQ180" t="n">
+        <v>0.1057739178256858</v>
+      </c>
     </row>
     <row r="181">
       <c r="A181" t="inlineStr">
@@ -22255,6 +23339,12 @@
       <c r="AM181" t="inlineStr"/>
       <c r="AN181" t="inlineStr"/>
       <c r="AO181" t="inlineStr"/>
+      <c r="AP181" t="n">
+        <v>0.4725159191080807</v>
+      </c>
+      <c r="AQ181" t="n">
+        <v>0.5647640205537345</v>
+      </c>
     </row>
     <row r="182">
       <c r="A182" t="inlineStr">
@@ -22380,6 +23470,12 @@
       <c r="AM182" t="inlineStr"/>
       <c r="AN182" t="inlineStr"/>
       <c r="AO182" t="inlineStr"/>
+      <c r="AP182" t="n">
+        <v>0.4336109424700468</v>
+      </c>
+      <c r="AQ182" t="n">
+        <v>0.5878104522136643</v>
+      </c>
     </row>
     <row r="183">
       <c r="A183" t="inlineStr">
@@ -22505,6 +23601,12 @@
       <c r="AM183" t="inlineStr"/>
       <c r="AN183" t="inlineStr"/>
       <c r="AO183" t="inlineStr"/>
+      <c r="AP183" t="n">
+        <v>0.4205663483021508</v>
+      </c>
+      <c r="AQ183" t="n">
+        <v>0.6067754159519365</v>
+      </c>
     </row>
     <row r="184">
       <c r="A184" t="inlineStr">
@@ -22626,6 +23728,12 @@
       <c r="AM184" t="inlineStr"/>
       <c r="AN184" t="inlineStr"/>
       <c r="AO184" t="inlineStr"/>
+      <c r="AP184" t="n">
+        <v>0.2738318531832623</v>
+      </c>
+      <c r="AQ184" t="n">
+        <v>0.4346384165069298</v>
+      </c>
     </row>
     <row r="185">
       <c r="A185" t="inlineStr">
@@ -22747,6 +23855,12 @@
       <c r="AM185" t="inlineStr"/>
       <c r="AN185" t="inlineStr"/>
       <c r="AO185" t="inlineStr"/>
+      <c r="AP185" t="n">
+        <v>0.4212719026278348</v>
+      </c>
+      <c r="AQ185" t="n">
+        <v>0.6151911445298365</v>
+      </c>
     </row>
     <row r="186">
       <c r="A186" t="inlineStr">
@@ -22872,6 +23986,12 @@
       <c r="AM186" t="inlineStr"/>
       <c r="AN186" t="inlineStr"/>
       <c r="AO186" t="inlineStr"/>
+      <c r="AP186" t="n">
+        <v>0.3017222602468082</v>
+      </c>
+      <c r="AQ186" t="n">
+        <v>0.5227134622483459</v>
+      </c>
     </row>
     <row r="187">
       <c r="A187" t="inlineStr">
@@ -22999,6 +24119,12 @@
       <c r="AM187" t="inlineStr"/>
       <c r="AN187" t="inlineStr"/>
       <c r="AO187" t="inlineStr"/>
+      <c r="AP187" t="n">
+        <v>0.1957528828104049</v>
+      </c>
+      <c r="AQ187" t="n">
+        <v>0.6384163711352652</v>
+      </c>
     </row>
     <row r="188">
       <c r="A188" t="inlineStr">
@@ -23110,6 +24236,12 @@
       <c r="AM188" t="inlineStr"/>
       <c r="AN188" t="inlineStr"/>
       <c r="AO188" t="inlineStr"/>
+      <c r="AP188" t="n">
+        <v>0.02291105121293801</v>
+      </c>
+      <c r="AQ188" t="n">
+        <v>0.0777906290570046</v>
+      </c>
     </row>
     <row r="189">
       <c r="A189" t="inlineStr">
@@ -23231,6 +24363,12 @@
       <c r="AM189" t="inlineStr"/>
       <c r="AN189" t="inlineStr"/>
       <c r="AO189" t="inlineStr"/>
+      <c r="AP189" t="n">
+        <v>0.0468384074941452</v>
+      </c>
+      <c r="AQ189" t="n">
+        <v>0.09460722477338826</v>
+      </c>
     </row>
     <row r="190">
       <c r="A190" t="inlineStr">
@@ -23354,6 +24492,12 @@
       <c r="AM190" t="inlineStr"/>
       <c r="AN190" t="inlineStr"/>
       <c r="AO190" t="inlineStr"/>
+      <c r="AP190" t="n">
+        <v>0.108060615550568</v>
+      </c>
+      <c r="AQ190" t="n">
+        <v>0.3413981663143849</v>
+      </c>
     </row>
     <row r="191">
       <c r="A191" t="inlineStr">
@@ -23473,6 +24617,12 @@
       <c r="AM191" t="inlineStr"/>
       <c r="AN191" t="inlineStr"/>
       <c r="AO191" t="inlineStr"/>
+      <c r="AP191" t="n">
+        <v>0.3146070269991933</v>
+      </c>
+      <c r="AQ191" t="n">
+        <v>0.396599979867541</v>
+      </c>
     </row>
     <row r="192">
       <c r="A192" t="inlineStr">
@@ -23600,6 +24750,12 @@
       <c r="AM192" t="inlineStr"/>
       <c r="AN192" t="inlineStr"/>
       <c r="AO192" t="inlineStr"/>
+      <c r="AP192" t="n">
+        <v>0.143482905982906</v>
+      </c>
+      <c r="AQ192" t="n">
+        <v>0.6866030804504873</v>
+      </c>
     </row>
     <row r="193">
       <c r="A193" t="inlineStr">
@@ -23715,6 +24871,12 @@
       <c r="AM193" t="inlineStr"/>
       <c r="AN193" t="inlineStr"/>
       <c r="AO193" t="inlineStr"/>
+      <c r="AP193" t="n">
+        <v>0.2796033416989386</v>
+      </c>
+      <c r="AQ193" t="n">
+        <v>0.3590984900897344</v>
+      </c>
     </row>
     <row r="194">
       <c r="A194" t="inlineStr">
@@ -23826,6 +24988,12 @@
       <c r="AM194" t="inlineStr"/>
       <c r="AN194" t="inlineStr"/>
       <c r="AO194" t="inlineStr"/>
+      <c r="AP194" t="n">
+        <v>0.560187333145301</v>
+      </c>
+      <c r="AQ194" t="n">
+        <v>0.6451090280335263</v>
+      </c>
     </row>
     <row r="195">
       <c r="A195" t="inlineStr">
@@ -23955,6 +25123,12 @@
       <c r="AM195" t="inlineStr"/>
       <c r="AN195" t="inlineStr"/>
       <c r="AO195" t="inlineStr"/>
+      <c r="AP195" t="n">
+        <v>0.6364977184366802</v>
+      </c>
+      <c r="AQ195" t="n">
+        <v>0.7177693142625931</v>
+      </c>
     </row>
     <row r="196">
       <c r="A196" t="inlineStr">
@@ -24072,6 +25246,12 @@
       <c r="AM196" t="inlineStr"/>
       <c r="AN196" t="inlineStr"/>
       <c r="AO196" t="inlineStr"/>
+      <c r="AP196" t="n">
+        <v>0.4477730061152708</v>
+      </c>
+      <c r="AQ196" t="n">
+        <v>0.5587078229099506</v>
+      </c>
     </row>
     <row r="197">
       <c r="A197" t="inlineStr">
@@ -24199,6 +25379,12 @@
       <c r="AM197" t="inlineStr"/>
       <c r="AN197" t="inlineStr"/>
       <c r="AO197" t="inlineStr"/>
+      <c r="AP197" t="n">
+        <v>0.3615904267689982</v>
+      </c>
+      <c r="AQ197" t="n">
+        <v>0.5480853091422807</v>
+      </c>
     </row>
     <row r="198">
       <c r="A198" t="inlineStr">
@@ -24324,6 +25510,12 @@
       <c r="AM198" t="inlineStr"/>
       <c r="AN198" t="inlineStr"/>
       <c r="AO198" t="inlineStr"/>
+      <c r="AP198" t="n">
+        <v>0.4266443976185084</v>
+      </c>
+      <c r="AQ198" t="n">
+        <v>0.6212772554887749</v>
+      </c>
     </row>
     <row r="199">
       <c r="A199" t="inlineStr">
@@ -24437,6 +25629,12 @@
       <c r="AM199" t="inlineStr"/>
       <c r="AN199" t="inlineStr"/>
       <c r="AO199" t="inlineStr"/>
+      <c r="AP199" t="n">
+        <v>0.0468384074941452</v>
+      </c>
+      <c r="AQ199" t="n">
+        <v>0.1096594270822946</v>
+      </c>
     </row>
     <row r="200">
       <c r="A200" t="inlineStr">
@@ -24562,6 +25760,12 @@
       <c r="AM200" t="inlineStr"/>
       <c r="AN200" t="inlineStr"/>
       <c r="AO200" t="inlineStr"/>
+      <c r="AP200" t="n">
+        <v>0.4153565160629284</v>
+      </c>
+      <c r="AQ200" t="n">
+        <v>0.6397492496642277</v>
+      </c>
     </row>
     <row r="201">
       <c r="A201" t="inlineStr">
@@ -24673,6 +25877,12 @@
       <c r="AM201" t="inlineStr"/>
       <c r="AN201" t="inlineStr"/>
       <c r="AO201" t="inlineStr"/>
+      <c r="AP201" t="n">
+        <v>0.5895268477438239</v>
+      </c>
+      <c r="AQ201" t="n">
+        <v>0.5990690742641294</v>
+      </c>
     </row>
     <row r="202">
       <c r="A202" t="inlineStr">
@@ -24800,6 +26010,12 @@
       <c r="AM202" t="inlineStr"/>
       <c r="AN202" t="inlineStr"/>
       <c r="AO202" t="inlineStr"/>
+      <c r="AP202" t="n">
+        <v>0.5954522266767165</v>
+      </c>
+      <c r="AQ202" t="n">
+        <v>0.650736752974502</v>
+      </c>
     </row>
     <row r="203">
       <c r="A203" t="inlineStr">
@@ -24925,6 +26141,12 @@
       <c r="AM203" t="inlineStr"/>
       <c r="AN203" t="inlineStr"/>
       <c r="AO203" t="inlineStr"/>
+      <c r="AP203" t="n">
+        <v>0.5660535578875775</v>
+      </c>
+      <c r="AQ203" t="n">
+        <v>0.6327792819321901</v>
+      </c>
     </row>
     <row r="204">
       <c r="A204" t="inlineStr">
@@ -25040,6 +26262,12 @@
       <c r="AM204" t="inlineStr"/>
       <c r="AN204" t="inlineStr"/>
       <c r="AO204" t="inlineStr"/>
+      <c r="AP204" t="n">
+        <v>0.6573429327214046</v>
+      </c>
+      <c r="AQ204" t="n">
+        <v>0.6552950403017638</v>
+      </c>
     </row>
     <row r="205">
       <c r="A205" t="inlineStr">
@@ -25167,6 +26395,12 @@
       <c r="AM205" t="inlineStr"/>
       <c r="AN205" t="inlineStr"/>
       <c r="AO205" t="inlineStr"/>
+      <c r="AP205" t="n">
+        <v>0.4522036803649155</v>
+      </c>
+      <c r="AQ205" t="n">
+        <v>0.6178883754483152</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>